<commit_message>
Fixed error with a lighting space type in a few rules. Changed from Dormitories to Guest Rooms
</commit_message>
<xml_diff>
--- a/rct229/ruletest_engine/ruletest_jsons/ruletest_spreadsheets/lighting_test_draft.xlsx
+++ b/rct229/ruletest_engine/ruletest_jsons/ruletest_spreadsheets/lighting_test_draft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ruleset-checking-tool\rct229\ruletest_engine\ruletest_jsons\ruletest_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{044A5367-4FD1-4241-A0E3-5993EEA6CE6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE069A2F-2D5B-41DF-A3CF-15A3BE33F724}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6D4BDC1E-634D-4FA4-9728-A76C548BE460}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="180">
   <si>
     <t>appendix_g_section_id</t>
   </si>
@@ -596,13 +596,16 @@
   </si>
   <si>
     <t>values</t>
+  </si>
+  <si>
+    <t>GUEST_ROOM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -646,12 +649,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -993,7 +990,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="185">
+  <dxfs count="183">
     <dxf>
       <fill>
         <patternFill>
@@ -1257,20 +1254,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2615,9 +2598,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD2616CE-C113-4173-BA9E-9D8DBBCAB481}">
   <dimension ref="A1:AO76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="5" topLeftCell="AH1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AJ61" sqref="AJ61"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3441,47 +3424,47 @@
       <c r="D8" s="12"/>
       <c r="E8" s="29"/>
       <c r="F8" s="6" t="str">
-        <f>"true"</f>
+        <f t="shared" ref="F8:P8" si="2">"true"</f>
         <v>true</v>
       </c>
       <c r="G8" s="6" t="str">
-        <f>"true"</f>
+        <f t="shared" si="2"/>
         <v>true</v>
       </c>
       <c r="H8" s="6" t="str">
-        <f>"true"</f>
+        <f t="shared" si="2"/>
         <v>true</v>
       </c>
       <c r="I8" s="6" t="str">
-        <f>"true"</f>
+        <f t="shared" si="2"/>
         <v>true</v>
       </c>
       <c r="J8" s="6" t="str">
-        <f>"true"</f>
+        <f t="shared" si="2"/>
         <v>true</v>
       </c>
       <c r="K8" s="6" t="str">
-        <f>"true"</f>
+        <f t="shared" si="2"/>
         <v>true</v>
       </c>
       <c r="L8" s="6" t="str">
-        <f>"true"</f>
+        <f t="shared" si="2"/>
         <v>true</v>
       </c>
       <c r="M8" s="6" t="str">
-        <f>"true"</f>
+        <f t="shared" si="2"/>
         <v>true</v>
       </c>
       <c r="N8" s="6" t="str">
-        <f>"true"</f>
+        <f t="shared" si="2"/>
         <v>true</v>
       </c>
       <c r="O8" s="6" t="str">
-        <f>"true"</f>
+        <f t="shared" si="2"/>
         <v>true</v>
       </c>
       <c r="P8" s="6" t="str">
-        <f>"true"</f>
+        <f t="shared" si="2"/>
         <v>true</v>
       </c>
       <c r="Q8" s="6"/>
@@ -3512,15 +3495,15 @@
         <v>true</v>
       </c>
       <c r="AC8" s="6" t="str">
-        <f t="shared" ref="AC8:AE8" si="2">"true"</f>
+        <f t="shared" ref="AC8:AE8" si="3">"true"</f>
         <v>true</v>
       </c>
       <c r="AD8" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>true</v>
       </c>
       <c r="AE8" s="6" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>true</v>
       </c>
       <c r="AF8" s="6"/>
@@ -3530,31 +3513,31 @@
         <v>true</v>
       </c>
       <c r="AI8" s="6" t="str">
-        <f t="shared" ref="AI8:AO8" si="3">"true"</f>
+        <f t="shared" ref="AI8:AO8" si="4">"true"</f>
         <v>true</v>
       </c>
       <c r="AJ8" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>true</v>
       </c>
       <c r="AK8" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>true</v>
       </c>
       <c r="AL8" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>true</v>
       </c>
       <c r="AM8" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>true</v>
       </c>
       <c r="AN8" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>true</v>
       </c>
       <c r="AO8" s="6" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>true</v>
       </c>
     </row>
@@ -4840,22 +4823,22 @@
       </c>
       <c r="E21" s="29"/>
       <c r="F21" s="35" t="s">
-        <v>81</v>
+        <v>179</v>
       </c>
       <c r="G21" s="35" t="s">
-        <v>81</v>
+        <v>179</v>
       </c>
       <c r="H21" s="35" t="s">
-        <v>81</v>
+        <v>179</v>
       </c>
       <c r="I21" s="35" t="s">
-        <v>81</v>
+        <v>179</v>
       </c>
       <c r="J21" s="35" t="s">
-        <v>81</v>
+        <v>179</v>
       </c>
       <c r="K21" s="35" t="s">
-        <v>81</v>
+        <v>179</v>
       </c>
       <c r="L21" s="27" t="s">
         <v>81</v>
@@ -6118,11 +6101,11 @@
         <v>SCHEDULE:CONSTANT-0.2055</v>
       </c>
       <c r="AN42" s="44" t="str">
-        <f t="shared" ref="AN42:AO42" si="4">"SCHEDULE:CONSTANT-"&amp;ROUND(1800/8760,4)</f>
+        <f t="shared" ref="AN42:AO42" si="5">"SCHEDULE:CONSTANT-"&amp;ROUND(1800/8760,4)</f>
         <v>SCHEDULE:CONSTANT-0.2055</v>
       </c>
       <c r="AO42" s="44" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>SCHEDULE:CONSTANT-0.2055</v>
       </c>
     </row>
@@ -7003,11 +6986,11 @@
         <v>SCHEDULE:CONSTANT-0.2671</v>
       </c>
       <c r="AI63" s="25" t="str">
-        <f t="shared" ref="AI63:AJ63" si="5">"SCHEDULE:CONSTANT-"&amp;ROUND(2340/8760,4)</f>
+        <f t="shared" ref="AI63:AJ63" si="6">"SCHEDULE:CONSTANT-"&amp;ROUND(2340/8760,4)</f>
         <v>SCHEDULE:CONSTANT-0.2671</v>
       </c>
       <c r="AJ63" s="25" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>SCHEDULE:CONSTANT-0.2671</v>
       </c>
       <c r="AL63" s="25" t="str">
@@ -7148,727 +7131,727 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A65:E76 A5:E5 A10:E18">
-    <cfRule type="expression" dxfId="184" priority="278">
+    <cfRule type="expression" dxfId="182" priority="278">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="expression" dxfId="183" priority="253">
+    <cfRule type="expression" dxfId="181" priority="253">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:E6">
-    <cfRule type="expression" dxfId="182" priority="252">
+    <cfRule type="expression" dxfId="180" priority="252">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="expression" dxfId="181" priority="250">
+    <cfRule type="expression" dxfId="179" priority="250">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:E9">
-    <cfRule type="expression" dxfId="180" priority="249">
+    <cfRule type="expression" dxfId="178" priority="249">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D57:E57">
-    <cfRule type="expression" dxfId="179" priority="266">
+    <cfRule type="expression" dxfId="177" priority="266">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C57">
-    <cfRule type="expression" dxfId="178" priority="265">
+    <cfRule type="expression" dxfId="176" priority="265">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="expression" dxfId="177" priority="251">
+    <cfRule type="expression" dxfId="175" priority="251">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58">
-    <cfRule type="expression" dxfId="176" priority="207">
+    <cfRule type="expression" dxfId="174" priority="207">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:B9">
-    <cfRule type="expression" dxfId="175" priority="236">
+    <cfRule type="expression" dxfId="173" priority="236">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22:E23">
-    <cfRule type="expression" dxfId="174" priority="247">
+    <cfRule type="expression" dxfId="172" priority="247">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21:E21">
-    <cfRule type="expression" dxfId="173" priority="238">
+    <cfRule type="expression" dxfId="171" priority="238">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D61:E61">
-    <cfRule type="expression" dxfId="172" priority="199">
+    <cfRule type="expression" dxfId="170" priority="199">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:B29 A22:B23">
-    <cfRule type="expression" dxfId="171" priority="237">
+    <cfRule type="expression" dxfId="169" priority="237">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:B21">
-    <cfRule type="expression" dxfId="170" priority="233">
+    <cfRule type="expression" dxfId="168" priority="233">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:B33">
-    <cfRule type="expression" dxfId="169" priority="234">
+    <cfRule type="expression" dxfId="167" priority="234">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:C23 C28:C36">
-    <cfRule type="expression" dxfId="168" priority="231">
+    <cfRule type="expression" dxfId="166" priority="231">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A57:B57">
-    <cfRule type="expression" dxfId="167" priority="232">
+    <cfRule type="expression" dxfId="165" priority="232">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D24:E25">
-    <cfRule type="expression" dxfId="166" priority="228">
+    <cfRule type="expression" dxfId="164" priority="228">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27:E27">
-    <cfRule type="expression" dxfId="165" priority="227">
+    <cfRule type="expression" dxfId="163" priority="227">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26:E26">
-    <cfRule type="expression" dxfId="164" priority="226">
+    <cfRule type="expression" dxfId="162" priority="226">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A27:B27 A24:B25">
-    <cfRule type="expression" dxfId="163" priority="225">
+    <cfRule type="expression" dxfId="161" priority="225">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:B26">
-    <cfRule type="expression" dxfId="162" priority="224">
+    <cfRule type="expression" dxfId="160" priority="224">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24:C27">
-    <cfRule type="expression" dxfId="161" priority="223">
+    <cfRule type="expression" dxfId="159" priority="223">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37:D38">
-    <cfRule type="expression" dxfId="160" priority="222">
+    <cfRule type="expression" dxfId="158" priority="222">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D59">
-    <cfRule type="expression" dxfId="159" priority="186">
+    <cfRule type="expression" dxfId="157" priority="186">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37:D38">
-    <cfRule type="expression" dxfId="158" priority="221">
+    <cfRule type="expression" dxfId="156" priority="221">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:B38">
-    <cfRule type="expression" dxfId="157" priority="219">
+    <cfRule type="expression" dxfId="155" priority="219">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C38">
-    <cfRule type="expression" dxfId="156" priority="217">
+    <cfRule type="expression" dxfId="154" priority="217">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37:E38">
-    <cfRule type="expression" dxfId="155" priority="216">
+    <cfRule type="expression" dxfId="153" priority="216">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28">
-    <cfRule type="expression" dxfId="154" priority="210">
+    <cfRule type="expression" dxfId="152" priority="210">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37">
-    <cfRule type="expression" dxfId="153" priority="215">
+    <cfRule type="expression" dxfId="151" priority="215">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28:D33">
-    <cfRule type="expression" dxfId="152" priority="213">
+    <cfRule type="expression" dxfId="150" priority="213">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28:D33">
-    <cfRule type="expression" dxfId="151" priority="212">
+    <cfRule type="expression" dxfId="149" priority="212">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28:E29">
-    <cfRule type="expression" dxfId="150" priority="211">
+    <cfRule type="expression" dxfId="148" priority="211">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30:E33">
-    <cfRule type="expression" dxfId="149" priority="209">
+    <cfRule type="expression" dxfId="147" priority="209">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E63">
-    <cfRule type="expression" dxfId="148" priority="197">
+    <cfRule type="expression" dxfId="146" priority="197">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D58:E58">
-    <cfRule type="expression" dxfId="147" priority="206">
+    <cfRule type="expression" dxfId="145" priority="206">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58:B58">
-    <cfRule type="expression" dxfId="146" priority="205">
+    <cfRule type="expression" dxfId="144" priority="205">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E60">
-    <cfRule type="expression" dxfId="145" priority="204">
+    <cfRule type="expression" dxfId="143" priority="204">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A59:B60">
-    <cfRule type="expression" dxfId="144" priority="202">
+    <cfRule type="expression" dxfId="142" priority="202">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A60:B60">
-    <cfRule type="expression" dxfId="143" priority="201">
+    <cfRule type="expression" dxfId="141" priority="201">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="expression" dxfId="142" priority="200">
+    <cfRule type="expression" dxfId="140" priority="200">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61:B61">
-    <cfRule type="expression" dxfId="141" priority="198">
+    <cfRule type="expression" dxfId="139" priority="198">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62:B63">
-    <cfRule type="expression" dxfId="140" priority="195">
+    <cfRule type="expression" dxfId="138" priority="195">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A63:B63">
-    <cfRule type="expression" dxfId="139" priority="194">
+    <cfRule type="expression" dxfId="137" priority="194">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C64">
-    <cfRule type="expression" dxfId="138" priority="193">
+    <cfRule type="expression" dxfId="136" priority="193">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D64:E64">
-    <cfRule type="expression" dxfId="137" priority="192">
+    <cfRule type="expression" dxfId="135" priority="192">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A64">
-    <cfRule type="expression" dxfId="136" priority="191">
+    <cfRule type="expression" dxfId="134" priority="191">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D62">
-    <cfRule type="expression" dxfId="135" priority="181">
+    <cfRule type="expression" dxfId="133" priority="181">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E62">
-    <cfRule type="expression" dxfId="134" priority="180">
+    <cfRule type="expression" dxfId="132" priority="180">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B64">
-    <cfRule type="expression" dxfId="133" priority="188">
+    <cfRule type="expression" dxfId="131" priority="188">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="expression" dxfId="132" priority="187">
+    <cfRule type="expression" dxfId="130" priority="187">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A36:B36">
-    <cfRule type="expression" dxfId="131" priority="176">
+    <cfRule type="expression" dxfId="129" priority="176">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D59">
-    <cfRule type="expression" dxfId="130" priority="185">
+    <cfRule type="expression" dxfId="128" priority="185">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E59">
-    <cfRule type="expression" dxfId="129" priority="184">
+    <cfRule type="expression" dxfId="127" priority="184">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="expression" dxfId="128" priority="183">
+    <cfRule type="expression" dxfId="126" priority="183">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D62">
-    <cfRule type="expression" dxfId="127" priority="182">
+    <cfRule type="expression" dxfId="125" priority="182">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51:B52">
-    <cfRule type="expression" dxfId="126" priority="115">
+    <cfRule type="expression" dxfId="124" priority="115">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A53:B54">
-    <cfRule type="expression" dxfId="125" priority="114">
+    <cfRule type="expression" dxfId="123" priority="114">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34:D36">
-    <cfRule type="expression" dxfId="124" priority="179">
+    <cfRule type="expression" dxfId="122" priority="179">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34:D36">
-    <cfRule type="expression" dxfId="123" priority="178">
+    <cfRule type="expression" dxfId="121" priority="178">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34:B35">
-    <cfRule type="expression" dxfId="122" priority="177">
+    <cfRule type="expression" dxfId="120" priority="177">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34">
-    <cfRule type="expression" dxfId="121" priority="173">
+    <cfRule type="expression" dxfId="119" priority="173">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E34:E35">
-    <cfRule type="expression" dxfId="120" priority="174">
+    <cfRule type="expression" dxfId="118" priority="174">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E36">
-    <cfRule type="expression" dxfId="119" priority="172">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F5:Z18 F21:Z27 F38:Z38 F34:I37 L34:Z37 F30:U33 F29:AA29 W30:AA33 AA21 AB29:AG33 AH29:AM29 AA10:AM18 F57:AM59 AN57:AO63 F64:AO76 F61:AM62 F60:AG60 AK60 F63:AG63 AK63">
-    <cfRule type="expression" dxfId="118" priority="169">
+    <cfRule type="expression" dxfId="117" priority="172">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5:Z18 F38:Z38 F34:I37 L34:Z37 F30:U33 F29:AA29 W30:AA33 AA21 AB29:AG33 AH29:AM29 AA10:AM18 F57:AM59 AN57:AO63 F64:AO76 F61:AM62 F60:AG60 AK60 F63:AG63 AK63 F21:Z27">
+    <cfRule type="expression" dxfId="116" priority="169">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C39:C42">
-    <cfRule type="expression" dxfId="117" priority="168">
+    <cfRule type="expression" dxfId="115" priority="168">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D39:E42">
-    <cfRule type="expression" dxfId="116" priority="167">
+    <cfRule type="expression" dxfId="114" priority="167">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:B42">
-    <cfRule type="expression" dxfId="115" priority="166">
+    <cfRule type="expression" dxfId="113" priority="166">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F39:Z42">
-    <cfRule type="expression" dxfId="114" priority="165">
+    <cfRule type="expression" dxfId="112" priority="165">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J34:K35">
-    <cfRule type="expression" dxfId="113" priority="164">
+    <cfRule type="expression" dxfId="111" priority="164">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA39:AG42">
-    <cfRule type="expression" dxfId="112" priority="160">
+    <cfRule type="expression" dxfId="110" priority="160">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J36:K37">
-    <cfRule type="expression" dxfId="111" priority="162">
+    <cfRule type="expression" dxfId="109" priority="162">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA34:AG38 AA5:AG9 AB21:AG21 AA22:AM27">
-    <cfRule type="expression" dxfId="110" priority="161">
+    <cfRule type="expression" dxfId="108" priority="161">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A43:B43">
-    <cfRule type="expression" dxfId="109" priority="159">
+    <cfRule type="expression" dxfId="107" priority="159">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C43:C47 C49">
-    <cfRule type="expression" dxfId="108" priority="158">
+    <cfRule type="expression" dxfId="106" priority="158">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19:E20">
-    <cfRule type="expression" dxfId="107" priority="130">
+    <cfRule type="expression" dxfId="105" priority="130">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49:B49">
-    <cfRule type="expression" dxfId="106" priority="155">
+    <cfRule type="expression" dxfId="104" priority="155">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C51:C56">
-    <cfRule type="expression" dxfId="105" priority="126">
+    <cfRule type="expression" dxfId="103" priority="126">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A55:B56">
-    <cfRule type="expression" dxfId="104" priority="123">
+    <cfRule type="expression" dxfId="102" priority="123">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D43">
-    <cfRule type="expression" dxfId="103" priority="151">
+    <cfRule type="expression" dxfId="101" priority="151">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D43">
-    <cfRule type="expression" dxfId="102" priority="150">
+    <cfRule type="expression" dxfId="100" priority="150">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43">
-    <cfRule type="expression" dxfId="101" priority="149">
+    <cfRule type="expression" dxfId="99" priority="149">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A46:B47">
-    <cfRule type="expression" dxfId="100" priority="145">
+    <cfRule type="expression" dxfId="98" priority="145">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D44:D45 D47">
-    <cfRule type="expression" dxfId="99" priority="148">
+    <cfRule type="expression" dxfId="97" priority="148">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D44:D45 D47">
-    <cfRule type="expression" dxfId="98" priority="147">
+    <cfRule type="expression" dxfId="96" priority="147">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A44:B45">
-    <cfRule type="expression" dxfId="97" priority="146">
+    <cfRule type="expression" dxfId="95" priority="146">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44">
-    <cfRule type="expression" dxfId="96" priority="143">
+    <cfRule type="expression" dxfId="94" priority="143">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44:E45">
-    <cfRule type="expression" dxfId="95" priority="144">
+    <cfRule type="expression" dxfId="93" priority="144">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E46:E47">
-    <cfRule type="expression" dxfId="94" priority="142">
+    <cfRule type="expression" dxfId="92" priority="142">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F56:Z56 F43:U43 W43:Y43 F44:I47 L44:Z47 L49:Z49 F49:I49">
-    <cfRule type="expression" dxfId="93" priority="141">
+    <cfRule type="expression" dxfId="91" priority="141">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J44:K45">
-    <cfRule type="expression" dxfId="92" priority="136">
+    <cfRule type="expression" dxfId="90" priority="136">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA44:AD46 AA47 AC47:AD47">
-    <cfRule type="expression" dxfId="91" priority="131">
+    <cfRule type="expression" dxfId="89" priority="131">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J46:K47 J49:K49">
-    <cfRule type="expression" dxfId="90" priority="135">
+    <cfRule type="expression" dxfId="88" priority="135">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA56:AG56 AA49:AD49 AF44:AG46 AF49:AG49 AF47">
-    <cfRule type="expression" dxfId="89" priority="134">
+    <cfRule type="expression" dxfId="87" priority="134">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D46">
-    <cfRule type="expression" dxfId="88" priority="132">
+    <cfRule type="expression" dxfId="86" priority="132">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH21">
-    <cfRule type="expression" dxfId="87" priority="59">
+    <cfRule type="expression" dxfId="85" priority="59">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F19:AM20">
-    <cfRule type="expression" dxfId="86" priority="129">
+    <cfRule type="expression" dxfId="84" priority="129">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB51:AD53 AC54">
-    <cfRule type="expression" dxfId="85" priority="103">
+    <cfRule type="expression" dxfId="83" priority="103">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C48">
-    <cfRule type="expression" dxfId="84" priority="102">
+    <cfRule type="expression" dxfId="82" priority="102">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A48:B48">
-    <cfRule type="expression" dxfId="83" priority="99">
+    <cfRule type="expression" dxfId="81" priority="99">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D48:D49">
-    <cfRule type="expression" dxfId="82" priority="93">
+    <cfRule type="expression" dxfId="80" priority="93">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D51:D52 D54">
-    <cfRule type="expression" dxfId="81" priority="117">
+    <cfRule type="expression" dxfId="79" priority="117">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D51:D52 D54">
-    <cfRule type="expression" dxfId="80" priority="116">
+    <cfRule type="expression" dxfId="78" priority="116">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
-    <cfRule type="expression" dxfId="79" priority="112">
+    <cfRule type="expression" dxfId="77" priority="112">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51:E52">
-    <cfRule type="expression" dxfId="78" priority="113">
+    <cfRule type="expression" dxfId="76" priority="113">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E53:E54">
-    <cfRule type="expression" dxfId="77" priority="111">
+    <cfRule type="expression" dxfId="75" priority="111">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F51:I55 L51:Z55">
-    <cfRule type="expression" dxfId="76" priority="110">
+    <cfRule type="expression" dxfId="74" priority="110">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J51:K52">
-    <cfRule type="expression" dxfId="75" priority="109">
+    <cfRule type="expression" dxfId="73" priority="109">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH50:AK50">
-    <cfRule type="expression" dxfId="74" priority="67">
+    <cfRule type="expression" dxfId="72" priority="67">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J53:K55">
-    <cfRule type="expression" dxfId="73" priority="108">
+    <cfRule type="expression" dxfId="71" priority="108">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA55:AF55 AE51:AF54 AG51:AG55">
-    <cfRule type="expression" dxfId="72" priority="107">
+    <cfRule type="expression" dxfId="70" priority="107">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D53">
-    <cfRule type="expression" dxfId="71" priority="106">
+    <cfRule type="expression" dxfId="69" priority="106">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA51:AA54">
-    <cfRule type="expression" dxfId="70" priority="104">
+    <cfRule type="expression" dxfId="68" priority="104">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH31:AM31">
-    <cfRule type="expression" dxfId="69" priority="66">
+    <cfRule type="expression" dxfId="67" priority="66">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L48:Z48 F48:I48">
-    <cfRule type="expression" dxfId="68" priority="96">
+    <cfRule type="expression" dxfId="66" priority="96">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J48:K48">
-    <cfRule type="expression" dxfId="67" priority="95">
+    <cfRule type="expression" dxfId="65" priority="95">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA48 AC48:AD48 AF48:AG48">
-    <cfRule type="expression" dxfId="66" priority="94">
+    <cfRule type="expression" dxfId="64" priority="94">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E48:E49">
-    <cfRule type="expression" dxfId="65" priority="92">
+    <cfRule type="expression" dxfId="63" priority="92">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D55:D56">
-    <cfRule type="expression" dxfId="64" priority="91">
+    <cfRule type="expression" dxfId="62" priority="91">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E55:E56">
-    <cfRule type="expression" dxfId="63" priority="90">
+    <cfRule type="expression" dxfId="61" priority="90">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C50">
-    <cfRule type="expression" dxfId="62" priority="89">
+    <cfRule type="expression" dxfId="60" priority="89">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50:B50">
-    <cfRule type="expression" dxfId="61" priority="88">
+    <cfRule type="expression" dxfId="59" priority="88">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L50:Z50 F50:I50">
-    <cfRule type="expression" dxfId="60" priority="87">
+    <cfRule type="expression" dxfId="58" priority="87">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J50:K50">
-    <cfRule type="expression" dxfId="59" priority="86">
+    <cfRule type="expression" dxfId="57" priority="86">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA50:AG50">
-    <cfRule type="expression" dxfId="58" priority="85">
+    <cfRule type="expression" dxfId="56" priority="85">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D50">
-    <cfRule type="expression" dxfId="57" priority="84">
+    <cfRule type="expression" dxfId="55" priority="84">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E50">
-    <cfRule type="expression" dxfId="56" priority="83">
+    <cfRule type="expression" dxfId="54" priority="83">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE44:AE47">
-    <cfRule type="expression" dxfId="55" priority="82">
+    <cfRule type="expression" dxfId="53" priority="82">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE49">
-    <cfRule type="expression" dxfId="54" priority="81">
+    <cfRule type="expression" dxfId="52" priority="81">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH32:AM33">
-    <cfRule type="expression" dxfId="53" priority="65">
+    <cfRule type="expression" dxfId="51" priority="65">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB48">
-    <cfRule type="expression" dxfId="52" priority="79">
+    <cfRule type="expression" dxfId="50" priority="79">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB54">
-    <cfRule type="expression" dxfId="51" priority="78">
+    <cfRule type="expression" dxfId="49" priority="78">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD54">
-    <cfRule type="expression" dxfId="50" priority="77">
+    <cfRule type="expression" dxfId="48" priority="77">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE48">
-    <cfRule type="expression" dxfId="49" priority="76">
+    <cfRule type="expression" dxfId="47" priority="76">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH30:AM30">
-    <cfRule type="expression" dxfId="48" priority="75">
+    <cfRule type="expression" dxfId="46" priority="75">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F41:AG41 AH39:AK40 F43:AK49 AL40:AM40 F42:AJ42">
-    <cfRule type="expression" dxfId="47" priority="73">
+    <cfRule type="expression" dxfId="45" priority="73">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH5:AK9 AH34:AK38">
-    <cfRule type="expression" dxfId="46" priority="74">
+    <cfRule type="expression" dxfId="44" priority="74">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH56:AK56 AH44:AK46 AH49:AK49">
-    <cfRule type="expression" dxfId="45" priority="72">
+    <cfRule type="expression" dxfId="43" priority="72">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH51:AK55">
-    <cfRule type="expression" dxfId="44" priority="69">
+    <cfRule type="expression" dxfId="42" priority="69">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH48:AK48">
-    <cfRule type="expression" dxfId="43" priority="68">
+    <cfRule type="expression" dxfId="41" priority="68">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL63">
-    <cfRule type="expression" dxfId="42" priority="7">
+    <cfRule type="expression" dxfId="40" priority="7">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="expression" dxfId="41" priority="64">
+    <cfRule type="expression" dxfId="39" priority="64">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63">
-    <cfRule type="expression" dxfId="39" priority="62">
+    <cfRule type="expression" dxfId="38" priority="62">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Made few corrections in lighting json and ruletest engine. Working to get Section6Rule1 running.
</commit_message>
<xml_diff>
--- a/rct229/ruletest_engine/ruletest_jsons/ruletest_spreadsheets/lighting_test_draft.xlsx
+++ b/rct229/ruletest_engine/ruletest_jsons/ruletest_spreadsheets/lighting_test_draft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ruleset-checking-tool\rct229\ruletest_engine\ruletest_jsons\ruletest_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF776F7-3434-4AB0-A524-DFC6CC002943}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B3A744-4FB7-4072-AB49-C37CC84D0246}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{6D4BDC1E-634D-4FA4-9728-A76C548BE460}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="170">
   <si>
     <t>appendix_g_section_id</t>
   </si>
@@ -970,7 +970,56 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="181">
+  <dxfs count="188">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2562,11 +2611,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD2616CE-C113-4173-BA9E-9D8DBBCAB481}">
-  <dimension ref="A1:AO77"/>
+  <dimension ref="A1:AO78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="5" topLeftCell="W1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W5" sqref="W5"/>
+      <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3342,8 +3391,12 @@
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
       <c r="E7" s="30"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
+      <c r="F7" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>68</v>
+      </c>
       <c r="H7" s="18"/>
       <c r="I7" s="18"/>
       <c r="J7" s="18"/>
@@ -3515,12 +3568,8 @@
       <c r="C9" s="21"/>
       <c r="D9" s="21"/>
       <c r="E9" s="31"/>
-      <c r="F9" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="G9" s="22" t="s">
-        <v>68</v>
-      </c>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
       <c r="H9" s="22" t="str">
         <f>"true"</f>
         <v>true</v>
@@ -3546,31 +3595,31 @@
       <c r="R9" s="22"/>
       <c r="S9" s="22"/>
       <c r="T9" s="22" t="str">
-        <f>"true"</f>
+        <f t="shared" ref="T9:Z9" si="5">"true"</f>
         <v>true</v>
       </c>
       <c r="U9" s="22" t="str">
-        <f>"true"</f>
+        <f t="shared" si="5"/>
         <v>true</v>
       </c>
       <c r="V9" s="22" t="str">
-        <f>"true"</f>
+        <f t="shared" si="5"/>
         <v>true</v>
       </c>
       <c r="W9" s="22" t="str">
-        <f>"true"</f>
+        <f t="shared" si="5"/>
         <v>true</v>
       </c>
       <c r="X9" s="22" t="str">
-        <f>"true"</f>
+        <f t="shared" si="5"/>
         <v>true</v>
       </c>
       <c r="Y9" s="22" t="str">
-        <f>"true"</f>
+        <f t="shared" si="5"/>
         <v>true</v>
       </c>
       <c r="Z9" s="22" t="str">
-        <f>"true"</f>
+        <f t="shared" si="5"/>
         <v>true</v>
       </c>
       <c r="AA9" s="22"/>
@@ -6215,11 +6264,11 @@
         <v>SCHEDULE:CONSTANT-0.2055</v>
       </c>
       <c r="AN43" s="44" t="str">
-        <f t="shared" ref="AN43:AO43" si="5">"SCHEDULE:CONSTANT-"&amp;ROUND(1800/8760,4)</f>
+        <f t="shared" ref="AN43:AO43" si="6">"SCHEDULE:CONSTANT-"&amp;ROUND(1800/8760,4)</f>
         <v>SCHEDULE:CONSTANT-0.2055</v>
       </c>
       <c r="AO43" s="44" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>SCHEDULE:CONSTANT-0.2055</v>
       </c>
     </row>
@@ -6894,89 +6943,91 @@
       <c r="B58" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C58" s="12"/>
-      <c r="D58" s="12"/>
-      <c r="E58" s="29"/>
+      <c r="C58" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D58" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E58" s="12" t="s">
+        <v>80</v>
+      </c>
       <c r="F58" s="6"/>
-      <c r="G58" s="6"/>
+      <c r="G58" s="6">
+        <v>0.51</v>
+      </c>
       <c r="H58" s="6"/>
       <c r="I58" s="6"/>
       <c r="J58" s="6"/>
       <c r="K58" s="6"/>
     </row>
-    <row r="59" spans="1:41" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="20" t="s">
+    <row r="59" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A59" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="B59" s="21" t="s">
+      <c r="B59" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C59" s="21"/>
-      <c r="D59" s="21"/>
-      <c r="E59" s="31"/>
-      <c r="F59" s="22"/>
-      <c r="G59" s="22"/>
-      <c r="H59" s="22"/>
-      <c r="I59" s="22"/>
-      <c r="J59" s="22"/>
-      <c r="K59" s="22"/>
-      <c r="L59" s="22"/>
-      <c r="M59" s="22"/>
-      <c r="N59" s="22"/>
-      <c r="O59" s="22"/>
-      <c r="P59" s="22"/>
-      <c r="Q59" s="22"/>
-      <c r="R59" s="22"/>
-      <c r="S59" s="22"/>
-      <c r="T59" s="22"/>
-      <c r="U59" s="22"/>
-      <c r="V59" s="22"/>
-      <c r="W59" s="22"/>
-      <c r="X59" s="22"/>
-      <c r="Y59" s="22"/>
-      <c r="Z59" s="22"/>
-      <c r="AA59" s="22"/>
-      <c r="AB59" s="22"/>
-      <c r="AC59" s="22"/>
-      <c r="AD59" s="22"/>
-      <c r="AE59" s="22"/>
-      <c r="AF59" s="22"/>
-      <c r="AG59" s="22"/>
-      <c r="AH59" s="22"/>
-      <c r="AI59" s="22"/>
-      <c r="AJ59" s="22"/>
-      <c r="AK59" s="22"/>
-      <c r="AL59" s="22"/>
-      <c r="AM59" s="22"/>
-      <c r="AN59" s="22"/>
-      <c r="AO59" s="22"/>
-    </row>
-    <row r="60" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A60" s="11" t="s">
+      <c r="C59" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D59" s="42" t="s">
+        <v>162</v>
+      </c>
+      <c r="E59" s="29"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="6"/>
+      <c r="H59" s="6"/>
+      <c r="I59" s="6"/>
+      <c r="J59" s="6"/>
+      <c r="K59" s="6"/>
+    </row>
+    <row r="60" spans="1:41" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="B60" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C60" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="D60" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="E60" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="F60" s="6"/>
-      <c r="G60" s="6">
-        <v>0.41</v>
-      </c>
-      <c r="H60" s="6"/>
-      <c r="I60" s="6">
-        <v>0.51</v>
-      </c>
-      <c r="J60" s="6"/>
-      <c r="K60" s="6"/>
+      <c r="B60" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C60" s="21"/>
+      <c r="D60" s="21"/>
+      <c r="E60" s="31"/>
+      <c r="F60" s="22"/>
+      <c r="G60" s="22"/>
+      <c r="H60" s="22"/>
+      <c r="I60" s="22"/>
+      <c r="J60" s="22"/>
+      <c r="K60" s="22"/>
+      <c r="L60" s="22"/>
+      <c r="M60" s="22"/>
+      <c r="N60" s="22"/>
+      <c r="O60" s="22"/>
+      <c r="P60" s="22"/>
+      <c r="Q60" s="22"/>
+      <c r="R60" s="22"/>
+      <c r="S60" s="22"/>
+      <c r="T60" s="22"/>
+      <c r="U60" s="22"/>
+      <c r="V60" s="22"/>
+      <c r="W60" s="22"/>
+      <c r="X60" s="22"/>
+      <c r="Y60" s="22"/>
+      <c r="Z60" s="22"/>
+      <c r="AA60" s="22"/>
+      <c r="AB60" s="22"/>
+      <c r="AC60" s="22"/>
+      <c r="AD60" s="22"/>
+      <c r="AE60" s="22"/>
+      <c r="AF60" s="22"/>
+      <c r="AG60" s="22"/>
+      <c r="AH60" s="22"/>
+      <c r="AI60" s="22"/>
+      <c r="AJ60" s="22"/>
+      <c r="AK60" s="22"/>
+      <c r="AL60" s="22"/>
+      <c r="AM60" s="22"/>
+      <c r="AN60" s="22"/>
+      <c r="AO60" s="22"/>
     </row>
     <row r="61" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A61" s="11" t="s">
@@ -6986,108 +7037,108 @@
         <v>12</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="D61" s="42" t="s">
-        <v>162</v>
-      </c>
-      <c r="E61" s="29"/>
+        <v>62</v>
+      </c>
+      <c r="D61" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E61" s="12" t="s">
+        <v>80</v>
+      </c>
       <c r="F61" s="6"/>
-      <c r="G61" s="6"/>
+      <c r="G61" s="6">
+        <v>0.41</v>
+      </c>
       <c r="H61" s="6"/>
-      <c r="I61" s="6"/>
+      <c r="I61" s="6">
+        <v>0.51</v>
+      </c>
       <c r="J61" s="6"/>
       <c r="K61" s="6"/>
-      <c r="AH61" s="25" t="str">
+    </row>
+    <row r="62" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A62" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B62" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C62" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D62" s="42" t="s">
+        <v>162</v>
+      </c>
+      <c r="E62" s="29"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
+      <c r="H62" s="6"/>
+      <c r="I62" s="6"/>
+      <c r="J62" s="6"/>
+      <c r="K62" s="6"/>
+      <c r="AH62" s="25" t="str">
         <f>"SCHEDULE:CONSTANT-"&amp;ROUND(1638/8760,4)</f>
         <v>SCHEDULE:CONSTANT-0.187</v>
       </c>
-      <c r="AI61" s="25" t="str">
+      <c r="AI62" s="25" t="str">
         <f>"SCHEDULE:CONSTANT-"&amp;ROUND(1900/8760,4)</f>
         <v>SCHEDULE:CONSTANT-0.2169</v>
       </c>
-      <c r="AJ61" s="25" t="str">
+      <c r="AJ62" s="25" t="str">
         <f>"SCHEDULE:CONSTANT-"&amp;ROUND(2400/8760,4)</f>
         <v>SCHEDULE:CONSTANT-0.274</v>
       </c>
-      <c r="AL61" s="25" t="str">
+      <c r="AL62" s="25" t="str">
         <f>"SCHEDULE:CONSTANT-"&amp;ROUND(1800/8760,4)</f>
         <v>SCHEDULE:CONSTANT-0.2055</v>
       </c>
     </row>
-    <row r="62" spans="1:41" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="20" t="s">
+    <row r="63" spans="1:41" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="B62" s="21" t="s">
+      <c r="B63" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C62" s="21"/>
-      <c r="D62" s="21"/>
-      <c r="E62" s="31"/>
-      <c r="F62" s="22"/>
-      <c r="G62" s="22"/>
-      <c r="H62" s="22"/>
-      <c r="I62" s="22"/>
-      <c r="J62" s="22"/>
-      <c r="K62" s="22"/>
-      <c r="L62" s="22"/>
-      <c r="M62" s="22"/>
-      <c r="N62" s="22"/>
-      <c r="O62" s="22"/>
-      <c r="P62" s="22"/>
-      <c r="Q62" s="22"/>
-      <c r="R62" s="22"/>
-      <c r="S62" s="22"/>
-      <c r="T62" s="22"/>
-      <c r="U62" s="22"/>
-      <c r="V62" s="22"/>
-      <c r="W62" s="22"/>
-      <c r="X62" s="22"/>
-      <c r="Y62" s="22"/>
-      <c r="Z62" s="22"/>
-      <c r="AA62" s="22"/>
-      <c r="AB62" s="22"/>
-      <c r="AC62" s="22"/>
-      <c r="AD62" s="22"/>
-      <c r="AE62" s="22"/>
-      <c r="AF62" s="22"/>
-      <c r="AG62" s="22"/>
-      <c r="AH62" s="22"/>
-      <c r="AI62" s="22"/>
-      <c r="AJ62" s="22"/>
-      <c r="AK62" s="22"/>
-      <c r="AL62" s="22"/>
-      <c r="AM62" s="22"/>
-      <c r="AN62" s="22"/>
-      <c r="AO62" s="22"/>
-    </row>
-    <row r="63" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A63" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B63" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="C63" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="D63" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="E63" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="F63" s="6"/>
-      <c r="G63" s="6">
-        <v>0.51</v>
-      </c>
-      <c r="H63" s="6"/>
-      <c r="I63" s="6">
-        <v>0.41</v>
-      </c>
-      <c r="J63" s="6"/>
-      <c r="K63" s="6"/>
+      <c r="C63" s="21"/>
+      <c r="D63" s="21"/>
+      <c r="E63" s="31"/>
+      <c r="F63" s="22"/>
+      <c r="G63" s="22"/>
+      <c r="H63" s="22"/>
+      <c r="I63" s="22"/>
+      <c r="J63" s="22"/>
+      <c r="K63" s="22"/>
+      <c r="L63" s="22"/>
+      <c r="M63" s="22"/>
+      <c r="N63" s="22"/>
+      <c r="O63" s="22"/>
+      <c r="P63" s="22"/>
+      <c r="Q63" s="22"/>
+      <c r="R63" s="22"/>
+      <c r="S63" s="22"/>
+      <c r="T63" s="22"/>
+      <c r="U63" s="22"/>
+      <c r="V63" s="22"/>
+      <c r="W63" s="22"/>
+      <c r="X63" s="22"/>
+      <c r="Y63" s="22"/>
+      <c r="Z63" s="22"/>
+      <c r="AA63" s="22"/>
+      <c r="AB63" s="22"/>
+      <c r="AC63" s="22"/>
+      <c r="AD63" s="22"/>
+      <c r="AE63" s="22"/>
+      <c r="AF63" s="22"/>
+      <c r="AG63" s="22"/>
+      <c r="AH63" s="22"/>
+      <c r="AI63" s="22"/>
+      <c r="AJ63" s="22"/>
+      <c r="AK63" s="22"/>
+      <c r="AL63" s="22"/>
+      <c r="AM63" s="22"/>
+      <c r="AN63" s="22"/>
+      <c r="AO63" s="22"/>
     </row>
     <row r="64" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A64" s="11" t="s">
@@ -7097,88 +7148,106 @@
         <v>11</v>
       </c>
       <c r="C64" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="D64" s="42" t="s">
-        <v>162</v>
-      </c>
-      <c r="E64" s="29"/>
+        <v>62</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E64" s="12" t="s">
+        <v>80</v>
+      </c>
       <c r="F64" s="6"/>
       <c r="G64" s="6"/>
       <c r="H64" s="6"/>
-      <c r="I64" s="6"/>
+      <c r="I64" s="6">
+        <v>0.41</v>
+      </c>
       <c r="J64" s="6"/>
       <c r="K64" s="6"/>
-      <c r="AH64" s="25" t="str">
+    </row>
+    <row r="65" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A65" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B65" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C65" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D65" s="42" t="s">
+        <v>162</v>
+      </c>
+      <c r="E65" s="29"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6"/>
+      <c r="H65" s="6"/>
+      <c r="I65" s="6"/>
+      <c r="J65" s="6"/>
+      <c r="K65" s="6"/>
+      <c r="AH65" s="25" t="str">
         <f>"SCHEDULE:CONSTANT-"&amp;ROUND(2340/8760,4)</f>
         <v>SCHEDULE:CONSTANT-0.2671</v>
       </c>
-      <c r="AI64" s="25" t="str">
-        <f t="shared" ref="AI64:AJ64" si="6">"SCHEDULE:CONSTANT-"&amp;ROUND(2340/8760,4)</f>
+      <c r="AI65" s="25" t="str">
+        <f t="shared" ref="AI65:AJ65" si="7">"SCHEDULE:CONSTANT-"&amp;ROUND(2340/8760,4)</f>
         <v>SCHEDULE:CONSTANT-0.2671</v>
       </c>
-      <c r="AJ64" s="25" t="str">
-        <f t="shared" si="6"/>
+      <c r="AJ65" s="25" t="str">
+        <f t="shared" si="7"/>
         <v>SCHEDULE:CONSTANT-0.2671</v>
       </c>
-      <c r="AL64" s="25" t="str">
+      <c r="AL65" s="25" t="str">
         <f>"SCHEDULE:CONSTANT-"&amp;ROUND(2000/8760,4)</f>
         <v>SCHEDULE:CONSTANT-0.2283</v>
       </c>
     </row>
-    <row r="65" spans="1:41" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="20" t="s">
+    <row r="66" spans="1:41" s="24" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="B65" s="20" t="s">
+      <c r="B66" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C65" s="21"/>
-      <c r="D65" s="21"/>
-      <c r="E65" s="31"/>
-      <c r="F65" s="22"/>
-      <c r="G65" s="22"/>
-      <c r="H65" s="22"/>
-      <c r="I65" s="22"/>
-      <c r="J65" s="22"/>
-      <c r="K65" s="22"/>
-      <c r="L65" s="22"/>
-      <c r="M65" s="22"/>
-      <c r="N65" s="22"/>
-      <c r="O65" s="22"/>
-      <c r="P65" s="22"/>
-      <c r="Q65" s="22"/>
-      <c r="R65" s="22"/>
-      <c r="S65" s="22"/>
-      <c r="T65" s="22"/>
-      <c r="U65" s="22"/>
-      <c r="V65" s="22"/>
-      <c r="W65" s="22"/>
-      <c r="X65" s="22"/>
-      <c r="Y65" s="22"/>
-      <c r="Z65" s="22"/>
-      <c r="AA65" s="22"/>
-      <c r="AB65" s="22"/>
-      <c r="AC65" s="22"/>
-      <c r="AD65" s="22"/>
-      <c r="AE65" s="22"/>
-      <c r="AF65" s="22"/>
-      <c r="AG65" s="22"/>
-      <c r="AH65" s="22"/>
-      <c r="AI65" s="22"/>
-      <c r="AJ65" s="22"/>
-      <c r="AK65" s="22"/>
-      <c r="AL65" s="22"/>
-      <c r="AM65" s="22"/>
-      <c r="AN65" s="22"/>
-      <c r="AO65" s="22"/>
-    </row>
-    <row r="66" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A66" s="11"/>
-      <c r="B66" s="12"/>
-      <c r="C66" s="12"/>
-      <c r="D66" s="12"/>
-      <c r="E66" s="29"/>
+      <c r="C66" s="21"/>
+      <c r="D66" s="21"/>
+      <c r="E66" s="31"/>
+      <c r="F66" s="22"/>
+      <c r="G66" s="22"/>
+      <c r="H66" s="22"/>
+      <c r="I66" s="22"/>
+      <c r="J66" s="22"/>
+      <c r="K66" s="22"/>
+      <c r="L66" s="22"/>
+      <c r="M66" s="22"/>
+      <c r="N66" s="22"/>
+      <c r="O66" s="22"/>
+      <c r="P66" s="22"/>
+      <c r="Q66" s="22"/>
+      <c r="R66" s="22"/>
+      <c r="S66" s="22"/>
+      <c r="T66" s="22"/>
+      <c r="U66" s="22"/>
+      <c r="V66" s="22"/>
+      <c r="W66" s="22"/>
+      <c r="X66" s="22"/>
+      <c r="Y66" s="22"/>
+      <c r="Z66" s="22"/>
+      <c r="AA66" s="22"/>
+      <c r="AB66" s="22"/>
+      <c r="AC66" s="22"/>
+      <c r="AD66" s="22"/>
+      <c r="AE66" s="22"/>
+      <c r="AF66" s="22"/>
+      <c r="AG66" s="22"/>
+      <c r="AH66" s="22"/>
+      <c r="AI66" s="22"/>
+      <c r="AJ66" s="22"/>
+      <c r="AK66" s="22"/>
+      <c r="AL66" s="22"/>
+      <c r="AM66" s="22"/>
+      <c r="AN66" s="22"/>
+      <c r="AO66" s="22"/>
     </row>
     <row r="67" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A67" s="11"/>
@@ -7257,908 +7326,940 @@
       <c r="D77" s="12"/>
       <c r="E77" s="29"/>
     </row>
+    <row r="78" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A78" s="11"/>
+      <c r="B78" s="12"/>
+      <c r="C78" s="12"/>
+      <c r="D78" s="12"/>
+      <c r="E78" s="29"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A66:E77 A5:E5 A10:E19">
-    <cfRule type="expression" dxfId="180" priority="278">
+  <conditionalFormatting sqref="A67:E78 A5:E5 A10:E19">
+    <cfRule type="expression" dxfId="187" priority="285">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="expression" dxfId="179" priority="253">
+    <cfRule type="expression" dxfId="186" priority="260">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:E6">
-    <cfRule type="expression" dxfId="178" priority="252">
+    <cfRule type="expression" dxfId="185" priority="259">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="expression" dxfId="177" priority="250">
+    <cfRule type="expression" dxfId="184" priority="257">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:E9">
-    <cfRule type="expression" dxfId="176" priority="249">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D58:E58">
-    <cfRule type="expression" dxfId="175" priority="266">
+    <cfRule type="expression" dxfId="183" priority="256">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6">
+    <cfRule type="expression" dxfId="180" priority="258">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C60">
+    <cfRule type="expression" dxfId="179" priority="214">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A7:B9">
+    <cfRule type="expression" dxfId="178" priority="243">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D23:E24">
+    <cfRule type="expression" dxfId="177" priority="254">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D22:E22">
+    <cfRule type="expression" dxfId="176" priority="245">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D63:E63">
+    <cfRule type="expression" dxfId="175" priority="206">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A29:B30 A23:B24">
+    <cfRule type="expression" dxfId="174" priority="244">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A22:B22">
+    <cfRule type="expression" dxfId="173" priority="240">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A31:B34">
+    <cfRule type="expression" dxfId="172" priority="241">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22:C24 C29:C37">
+    <cfRule type="expression" dxfId="171" priority="238">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A58:B59">
+    <cfRule type="expression" dxfId="170" priority="239">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D25:E26">
+    <cfRule type="expression" dxfId="169" priority="235">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D28:E28">
+    <cfRule type="expression" dxfId="168" priority="234">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27:E27">
+    <cfRule type="expression" dxfId="167" priority="233">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A28:B28 A25:B26">
+    <cfRule type="expression" dxfId="166" priority="232">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A27:B27">
+    <cfRule type="expression" dxfId="165" priority="231">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C25:C28">
+    <cfRule type="expression" dxfId="164" priority="230">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38:D39">
+    <cfRule type="expression" dxfId="163" priority="229">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D61">
+    <cfRule type="expression" dxfId="162" priority="193">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38:D39">
+    <cfRule type="expression" dxfId="161" priority="228">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A38:B39">
+    <cfRule type="expression" dxfId="160" priority="226">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C39">
+    <cfRule type="expression" dxfId="159" priority="224">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E38:E39">
+    <cfRule type="expression" dxfId="158" priority="223">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E29">
+    <cfRule type="expression" dxfId="157" priority="217">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E38">
+    <cfRule type="expression" dxfId="156" priority="222">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D29:D34">
+    <cfRule type="expression" dxfId="155" priority="220">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D29:D34">
+    <cfRule type="expression" dxfId="154" priority="219">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E29:E30">
+    <cfRule type="expression" dxfId="153" priority="218">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31:E34">
+    <cfRule type="expression" dxfId="152" priority="216">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E65">
+    <cfRule type="expression" dxfId="151" priority="204">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D60:E60">
+    <cfRule type="expression" dxfId="150" priority="213">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A60:B60">
+    <cfRule type="expression" dxfId="149" priority="212">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E62">
+    <cfRule type="expression" dxfId="148" priority="211">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A61:B62">
+    <cfRule type="expression" dxfId="147" priority="209">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A62:B62">
+    <cfRule type="expression" dxfId="146" priority="208">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C63">
+    <cfRule type="expression" dxfId="145" priority="207">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A63:B63">
+    <cfRule type="expression" dxfId="144" priority="205">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A64:B65">
+    <cfRule type="expression" dxfId="143" priority="202">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A65:B65">
+    <cfRule type="expression" dxfId="142" priority="201">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C66">
+    <cfRule type="expression" dxfId="141" priority="200">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D66:E66">
+    <cfRule type="expression" dxfId="140" priority="199">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A66">
+    <cfRule type="expression" dxfId="139" priority="198">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D64">
+    <cfRule type="expression" dxfId="138" priority="188">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E64">
+    <cfRule type="expression" dxfId="137" priority="187">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B66">
+    <cfRule type="expression" dxfId="136" priority="195">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
+    <cfRule type="expression" dxfId="135" priority="194">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37:B37">
+    <cfRule type="expression" dxfId="134" priority="183">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D61">
+    <cfRule type="expression" dxfId="133" priority="192">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E61">
+    <cfRule type="expression" dxfId="132" priority="191">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C64">
+    <cfRule type="expression" dxfId="131" priority="190">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D64">
+    <cfRule type="expression" dxfId="130" priority="189">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A52:B53">
+    <cfRule type="expression" dxfId="129" priority="122">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A54:B55">
+    <cfRule type="expression" dxfId="128" priority="121">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35:D37">
+    <cfRule type="expression" dxfId="127" priority="186">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35:D37">
+    <cfRule type="expression" dxfId="126" priority="185">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A35:B36">
+    <cfRule type="expression" dxfId="125" priority="184">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E35">
+    <cfRule type="expression" dxfId="124" priority="180">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E35:E36">
+    <cfRule type="expression" dxfId="123" priority="181">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E37">
+    <cfRule type="expression" dxfId="122" priority="179">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F35:K38 AA22 AH30:AM30 AA10:AM13 AN58:AO65 AK62 AK65 V35:Z43 V58:AM61 V66:AO78 V63:AM64 V62:AG62 V65:AG65 V22:Z28 V5:Z13 V15:AM21 V14:AO14 V51:Z57 V42:AG42 V43:AJ43 V44:AK50 F39:U50 N35:U38 N51:U56 W35:W78 W5:W28 R35:U78 Y35:Y78 F30:AG34 Y5:Y28 F5:U28 F57:U78">
+    <cfRule type="expression" dxfId="121" priority="176">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40:C43">
+    <cfRule type="expression" dxfId="120" priority="175">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40:E43">
+    <cfRule type="expression" dxfId="119" priority="174">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A40:B43">
+    <cfRule type="expression" dxfId="118" priority="173">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L35:M36">
+    <cfRule type="expression" dxfId="117" priority="171">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA40:AG43">
+    <cfRule type="expression" dxfId="116" priority="167">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L37:M38">
+    <cfRule type="expression" dxfId="115" priority="169">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA35:AG39 AA5:AG9 AB22:AG22 AA23:AM28">
+    <cfRule type="expression" dxfId="114" priority="168">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A44:B44">
+    <cfRule type="expression" dxfId="113" priority="166">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C44:C48 C50">
+    <cfRule type="expression" dxfId="112" priority="165">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A20:E21">
+    <cfRule type="expression" dxfId="111" priority="137">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A50:B50">
+    <cfRule type="expression" dxfId="110" priority="162">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C52:C57">
+    <cfRule type="expression" dxfId="109" priority="133">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A56:B57">
+    <cfRule type="expression" dxfId="108" priority="130">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D44">
+    <cfRule type="expression" dxfId="107" priority="158">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D44">
+    <cfRule type="expression" dxfId="106" priority="157">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E44">
+    <cfRule type="expression" dxfId="105" priority="156">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A47:B48">
+    <cfRule type="expression" dxfId="104" priority="152">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D45:D46 D48">
+    <cfRule type="expression" dxfId="103" priority="155">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D45:D46 D48">
+    <cfRule type="expression" dxfId="102" priority="154">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A45:B46">
+    <cfRule type="expression" dxfId="101" priority="153">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E45">
+    <cfRule type="expression" dxfId="100" priority="150">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E45:E46">
+    <cfRule type="expression" dxfId="99" priority="151">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E47:E48">
+    <cfRule type="expression" dxfId="98" priority="149">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F45:K48 F50:K50">
+    <cfRule type="expression" dxfId="97" priority="148">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L45:M46">
+    <cfRule type="expression" dxfId="96" priority="143">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA45:AD47 AA48 AC48:AD48">
+    <cfRule type="expression" dxfId="95" priority="138">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L47:M48 L50:M50">
+    <cfRule type="expression" dxfId="94" priority="142">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA57:AG57 AA50:AD50 AF45:AG47 AF50:AG50 AF48">
+    <cfRule type="expression" dxfId="93" priority="141">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D47">
+    <cfRule type="expression" dxfId="92" priority="139">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH22">
+    <cfRule type="expression" dxfId="91" priority="66">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB52:AD54 AC55">
+    <cfRule type="expression" dxfId="90" priority="110">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C49">
+    <cfRule type="expression" dxfId="89" priority="109">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A49:B49">
+    <cfRule type="expression" dxfId="88" priority="106">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D49:D50">
+    <cfRule type="expression" dxfId="87" priority="100">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D52:D53 D55">
+    <cfRule type="expression" dxfId="86" priority="124">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D52:D53 D55">
+    <cfRule type="expression" dxfId="85" priority="123">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E52">
+    <cfRule type="expression" dxfId="84" priority="119">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E52:E53">
+    <cfRule type="expression" dxfId="83" priority="120">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E54:E55">
+    <cfRule type="expression" dxfId="82" priority="118">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F52:K56">
+    <cfRule type="expression" dxfId="81" priority="117">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L52:M53">
+    <cfRule type="expression" dxfId="80" priority="116">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH51:AK51">
+    <cfRule type="expression" dxfId="79" priority="74">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L54:M56">
+    <cfRule type="expression" dxfId="78" priority="115">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA56:AF56 AE52:AF55 AG52:AG56">
+    <cfRule type="expression" dxfId="77" priority="114">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D54">
+    <cfRule type="expression" dxfId="76" priority="113">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA52:AA55">
+    <cfRule type="expression" dxfId="75" priority="111">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH32:AM32">
+    <cfRule type="expression" dxfId="74" priority="73">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F49:K49">
+    <cfRule type="expression" dxfId="73" priority="103">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L49:M49">
+    <cfRule type="expression" dxfId="72" priority="102">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA49 AC49:AD49 AF49:AG49">
+    <cfRule type="expression" dxfId="71" priority="101">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E49:E50">
+    <cfRule type="expression" dxfId="70" priority="99">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D56:D57">
+    <cfRule type="expression" dxfId="69" priority="98">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E56:E57">
+    <cfRule type="expression" dxfId="68" priority="97">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="expression" dxfId="67" priority="96">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A51:B51">
+    <cfRule type="expression" dxfId="66" priority="95">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F51:K51">
+    <cfRule type="expression" dxfId="65" priority="94">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L51:M51">
+    <cfRule type="expression" dxfId="64" priority="93">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA51:AG51">
+    <cfRule type="expression" dxfId="63" priority="92">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D51">
+    <cfRule type="expression" dxfId="62" priority="91">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E51">
+    <cfRule type="expression" dxfId="61" priority="90">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE45:AE48">
+    <cfRule type="expression" dxfId="60" priority="89">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE50">
+    <cfRule type="expression" dxfId="59" priority="88">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH33:AM34">
+    <cfRule type="expression" dxfId="58" priority="72">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB49">
+    <cfRule type="expression" dxfId="57" priority="86">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB55">
+    <cfRule type="expression" dxfId="56" priority="85">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD55">
+    <cfRule type="expression" dxfId="55" priority="84">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE49">
+    <cfRule type="expression" dxfId="54" priority="83">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH31:AM31">
+    <cfRule type="expression" dxfId="53" priority="82">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH40:AK41 AL41:AM41">
+    <cfRule type="expression" dxfId="52" priority="80">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH5:AK9 AH35:AK39">
+    <cfRule type="expression" dxfId="51" priority="81">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH57:AK57 AH45:AK47 AH50:AK50">
+    <cfRule type="expression" dxfId="50" priority="79">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH52:AK56">
+    <cfRule type="expression" dxfId="49" priority="76">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH49:AK49">
+    <cfRule type="expression" dxfId="48" priority="75">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL65">
+    <cfRule type="expression" dxfId="47" priority="14">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C62">
+    <cfRule type="expression" dxfId="46" priority="71">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C65">
+    <cfRule type="expression" dxfId="45" priority="69">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH42:AM42">
+    <cfRule type="expression" dxfId="44" priority="67">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI22:AM22">
+    <cfRule type="expression" dxfId="43" priority="65">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL51:AM51">
+    <cfRule type="expression" dxfId="42" priority="54">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM43:AO43">
+    <cfRule type="expression" dxfId="41" priority="17">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK43">
+    <cfRule type="expression" dxfId="40" priority="16">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL40:AM40 AL44:AM50 AL43">
+    <cfRule type="expression" dxfId="39" priority="59">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL5:AM9 AL35:AM39 AM62 AM65">
+    <cfRule type="expression" dxfId="38" priority="60">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL57:AM57 AL45:AM47 AL50:AM50">
+    <cfRule type="expression" dxfId="37" priority="58">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL52:AM56">
+    <cfRule type="expression" dxfId="36" priority="56">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL49:AM49">
+    <cfRule type="expression" dxfId="35" priority="55">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL62">
+    <cfRule type="expression" dxfId="34" priority="15">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AN30:AO30 AN10:AO13 AN15:AO19">
+    <cfRule type="expression" dxfId="33" priority="49">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AN23:AO28">
+    <cfRule type="expression" dxfId="32" priority="48">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AN20:AO21">
+    <cfRule type="expression" dxfId="31" priority="47">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AN32:AO32">
+    <cfRule type="expression" dxfId="30" priority="44">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AN33:AO34">
+    <cfRule type="expression" dxfId="29" priority="43">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AN31:AO31">
+    <cfRule type="expression" dxfId="28" priority="46">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AN41:AO41">
+    <cfRule type="expression" dxfId="27" priority="45">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AN42:AO42">
+    <cfRule type="expression" dxfId="26" priority="42">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AN22:AO22">
+    <cfRule type="expression" dxfId="25" priority="41">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AN51">
+    <cfRule type="expression" dxfId="24" priority="34">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AN44:AN50 AN40:AO40">
+    <cfRule type="expression" dxfId="23" priority="39">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AN5:AN9 AO8:AO9 AN35:AO39">
+    <cfRule type="expression" dxfId="22" priority="40">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AN57 AN45:AN47 AN50">
+    <cfRule type="expression" dxfId="21" priority="38">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AN52:AN56">
+    <cfRule type="expression" dxfId="20" priority="36">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AN49">
+    <cfRule type="expression" dxfId="19" priority="35">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AO5:AO7">
+    <cfRule type="expression" dxfId="18" priority="24">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AO44:AO50">
+    <cfRule type="expression" dxfId="17" priority="23">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AO57 AO45:AO47 AO50">
+    <cfRule type="expression" dxfId="16" priority="22">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AO51">
+    <cfRule type="expression" dxfId="15" priority="18">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AO52:AO56">
+    <cfRule type="expression" dxfId="14" priority="20">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AO49">
+    <cfRule type="expression" dxfId="13" priority="19">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D62">
+    <cfRule type="expression" dxfId="12" priority="13">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D65">
+    <cfRule type="expression" dxfId="11" priority="12">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH62">
+    <cfRule type="expression" dxfId="10" priority="11">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH65:AJ65">
+    <cfRule type="expression" dxfId="9" priority="10">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI62">
+    <cfRule type="expression" dxfId="8" priority="9">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ62">
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D58">
+    <cfRule type="expression" dxfId="6" priority="5">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E59">
+    <cfRule type="expression" dxfId="5" priority="7">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C58">
-    <cfRule type="expression" dxfId="174" priority="265">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A6">
-    <cfRule type="expression" dxfId="173" priority="251">
+    <cfRule type="expression" dxfId="4" priority="6">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D58">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E58">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="expression" dxfId="172" priority="207">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A7:B9">
-    <cfRule type="expression" dxfId="171" priority="236">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D23:E24">
-    <cfRule type="expression" dxfId="170" priority="247">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D22:E22">
-    <cfRule type="expression" dxfId="169" priority="238">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D62:E62">
-    <cfRule type="expression" dxfId="168" priority="199">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A29:B30 A23:B24">
-    <cfRule type="expression" dxfId="167" priority="237">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A22:B22">
-    <cfRule type="expression" dxfId="166" priority="233">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A31:B34">
-    <cfRule type="expression" dxfId="165" priority="234">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C22:C24 C29:C37">
-    <cfRule type="expression" dxfId="164" priority="231">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A58:B58">
-    <cfRule type="expression" dxfId="163" priority="232">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D25:E26">
-    <cfRule type="expression" dxfId="162" priority="228">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D28:E28">
-    <cfRule type="expression" dxfId="161" priority="227">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D27:E27">
-    <cfRule type="expression" dxfId="160" priority="226">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A28:B28 A25:B26">
-    <cfRule type="expression" dxfId="159" priority="225">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A27:B27">
-    <cfRule type="expression" dxfId="158" priority="224">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C25:C28">
-    <cfRule type="expression" dxfId="157" priority="223">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D38:D39">
-    <cfRule type="expression" dxfId="156" priority="222">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D60">
-    <cfRule type="expression" dxfId="155" priority="186">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D38:D39">
-    <cfRule type="expression" dxfId="154" priority="221">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A38:B39">
-    <cfRule type="expression" dxfId="153" priority="219">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C39">
-    <cfRule type="expression" dxfId="152" priority="217">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E38:E39">
-    <cfRule type="expression" dxfId="151" priority="216">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E29">
-    <cfRule type="expression" dxfId="150" priority="210">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E38">
-    <cfRule type="expression" dxfId="149" priority="215">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D29:D34">
-    <cfRule type="expression" dxfId="148" priority="213">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D29:D34">
-    <cfRule type="expression" dxfId="147" priority="212">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E29:E30">
-    <cfRule type="expression" dxfId="146" priority="211">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E31:E34">
-    <cfRule type="expression" dxfId="145" priority="209">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E64">
-    <cfRule type="expression" dxfId="144" priority="197">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D59:E59">
-    <cfRule type="expression" dxfId="143" priority="206">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A59:B59">
-    <cfRule type="expression" dxfId="142" priority="205">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E61">
-    <cfRule type="expression" dxfId="141" priority="204">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A60:B61">
-    <cfRule type="expression" dxfId="140" priority="202">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A61:B61">
-    <cfRule type="expression" dxfId="139" priority="201">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C62">
-    <cfRule type="expression" dxfId="138" priority="200">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A62:B62">
-    <cfRule type="expression" dxfId="137" priority="198">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A63:B64">
-    <cfRule type="expression" dxfId="136" priority="195">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A64:B64">
-    <cfRule type="expression" dxfId="135" priority="194">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C65">
-    <cfRule type="expression" dxfId="134" priority="193">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D65:E65">
-    <cfRule type="expression" dxfId="133" priority="192">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A65">
-    <cfRule type="expression" dxfId="132" priority="191">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D63">
-    <cfRule type="expression" dxfId="131" priority="181">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E63">
-    <cfRule type="expression" dxfId="130" priority="180">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B65">
-    <cfRule type="expression" dxfId="129" priority="188">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
-    <cfRule type="expression" dxfId="128" priority="187">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A37:B37">
-    <cfRule type="expression" dxfId="127" priority="176">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D60">
-    <cfRule type="expression" dxfId="126" priority="185">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E60">
-    <cfRule type="expression" dxfId="125" priority="184">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="expression" dxfId="124" priority="183">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D63">
-    <cfRule type="expression" dxfId="123" priority="182">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A52:B53">
-    <cfRule type="expression" dxfId="122" priority="115">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A54:B55">
-    <cfRule type="expression" dxfId="121" priority="114">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D35:D37">
-    <cfRule type="expression" dxfId="120" priority="179">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D35:D37">
-    <cfRule type="expression" dxfId="119" priority="178">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A35:B36">
-    <cfRule type="expression" dxfId="118" priority="177">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E35">
-    <cfRule type="expression" dxfId="117" priority="173">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E35:E36">
-    <cfRule type="expression" dxfId="116" priority="174">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E37">
-    <cfRule type="expression" dxfId="115" priority="172">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F35:K38 AA22 AH30:AM30 AA10:AM13 AN58:AO64 AK61 AK64 V35:Z43 V58:AM60 V65:AO77 V62:AM63 V61:AG61 V64:AG64 V22:Z28 V5:Z13 V15:AM21 V14:AO14 V51:Z57 V42:AG42 V43:AJ43 V44:AK50 F39:U50 N35:U38 F57:U77 N51:U56 W35:W77 W5:W28 R35:U77 Y35:Y77 F30:AG34 F5:U28 Y5:Y28">
-    <cfRule type="expression" dxfId="114" priority="169">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C40:C43">
-    <cfRule type="expression" dxfId="113" priority="168">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D40:E43">
-    <cfRule type="expression" dxfId="112" priority="167">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A40:B43">
-    <cfRule type="expression" dxfId="111" priority="166">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L35:M36">
-    <cfRule type="expression" dxfId="110" priority="164">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA40:AG43">
-    <cfRule type="expression" dxfId="109" priority="160">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L37:M38">
-    <cfRule type="expression" dxfId="108" priority="162">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA35:AG39 AA5:AG9 AB22:AG22 AA23:AM28">
-    <cfRule type="expression" dxfId="107" priority="161">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A44:B44">
-    <cfRule type="expression" dxfId="106" priority="159">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C44:C48 C50">
-    <cfRule type="expression" dxfId="105" priority="158">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A20:E21">
-    <cfRule type="expression" dxfId="104" priority="130">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A50:B50">
-    <cfRule type="expression" dxfId="103" priority="155">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C52:C57">
-    <cfRule type="expression" dxfId="102" priority="126">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A56:B57">
-    <cfRule type="expression" dxfId="101" priority="123">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D44">
-    <cfRule type="expression" dxfId="100" priority="151">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D44">
-    <cfRule type="expression" dxfId="99" priority="150">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E44">
-    <cfRule type="expression" dxfId="98" priority="149">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A47:B48">
-    <cfRule type="expression" dxfId="97" priority="145">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D45:D46 D48">
-    <cfRule type="expression" dxfId="96" priority="148">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D45:D46 D48">
-    <cfRule type="expression" dxfId="95" priority="147">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A45:B46">
-    <cfRule type="expression" dxfId="94" priority="146">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E45">
-    <cfRule type="expression" dxfId="93" priority="143">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E45:E46">
-    <cfRule type="expression" dxfId="92" priority="144">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E47:E48">
-    <cfRule type="expression" dxfId="91" priority="142">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F45:K48 F50:K50">
-    <cfRule type="expression" dxfId="90" priority="141">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L45:M46">
-    <cfRule type="expression" dxfId="89" priority="136">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA45:AD47 AA48 AC48:AD48">
-    <cfRule type="expression" dxfId="88" priority="131">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L47:M48 L50:M50">
-    <cfRule type="expression" dxfId="87" priority="135">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA57:AG57 AA50:AD50 AF45:AG47 AF50:AG50 AF48">
-    <cfRule type="expression" dxfId="86" priority="134">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D47">
-    <cfRule type="expression" dxfId="85" priority="132">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH22">
-    <cfRule type="expression" dxfId="84" priority="59">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB52:AD54 AC55">
-    <cfRule type="expression" dxfId="83" priority="103">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
-    <cfRule type="expression" dxfId="82" priority="102">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A49:B49">
-    <cfRule type="expression" dxfId="81" priority="99">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D49:D50">
-    <cfRule type="expression" dxfId="80" priority="93">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D52:D53 D55">
-    <cfRule type="expression" dxfId="79" priority="117">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D52:D53 D55">
-    <cfRule type="expression" dxfId="78" priority="116">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E52">
-    <cfRule type="expression" dxfId="77" priority="112">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E52:E53">
-    <cfRule type="expression" dxfId="76" priority="113">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E54:E55">
-    <cfRule type="expression" dxfId="75" priority="111">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F52:K56">
-    <cfRule type="expression" dxfId="74" priority="110">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L52:M53">
-    <cfRule type="expression" dxfId="73" priority="109">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH51:AK51">
-    <cfRule type="expression" dxfId="72" priority="67">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L54:M56">
-    <cfRule type="expression" dxfId="71" priority="108">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA56:AF56 AE52:AF55 AG52:AG56">
-    <cfRule type="expression" dxfId="70" priority="107">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D54">
-    <cfRule type="expression" dxfId="69" priority="106">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA52:AA55">
-    <cfRule type="expression" dxfId="68" priority="104">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH32:AM32">
-    <cfRule type="expression" dxfId="67" priority="66">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F49:K49">
-    <cfRule type="expression" dxfId="66" priority="96">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L49:M49">
-    <cfRule type="expression" dxfId="65" priority="95">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA49 AC49:AD49 AF49:AG49">
-    <cfRule type="expression" dxfId="64" priority="94">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E49:E50">
-    <cfRule type="expression" dxfId="63" priority="92">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D56:D57">
-    <cfRule type="expression" dxfId="62" priority="91">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E56:E57">
-    <cfRule type="expression" dxfId="61" priority="90">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="expression" dxfId="60" priority="89">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A51:B51">
-    <cfRule type="expression" dxfId="59" priority="88">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F51:K51">
-    <cfRule type="expression" dxfId="58" priority="87">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L51:M51">
-    <cfRule type="expression" dxfId="57" priority="86">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA51:AG51">
-    <cfRule type="expression" dxfId="56" priority="85">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D51">
-    <cfRule type="expression" dxfId="55" priority="84">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E51">
-    <cfRule type="expression" dxfId="54" priority="83">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE45:AE48">
-    <cfRule type="expression" dxfId="53" priority="82">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE50">
-    <cfRule type="expression" dxfId="52" priority="81">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH33:AM34">
-    <cfRule type="expression" dxfId="51" priority="65">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB49">
-    <cfRule type="expression" dxfId="50" priority="79">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB55">
-    <cfRule type="expression" dxfId="49" priority="78">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD55">
-    <cfRule type="expression" dxfId="48" priority="77">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE49">
-    <cfRule type="expression" dxfId="47" priority="76">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH31:AM31">
-    <cfRule type="expression" dxfId="46" priority="75">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH40:AK41 AL41:AM41">
-    <cfRule type="expression" dxfId="45" priority="73">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH5:AK9 AH35:AK39">
-    <cfRule type="expression" dxfId="44" priority="74">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH57:AK57 AH45:AK47 AH50:AK50">
-    <cfRule type="expression" dxfId="43" priority="72">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH52:AK56">
-    <cfRule type="expression" dxfId="42" priority="69">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH49:AK49">
-    <cfRule type="expression" dxfId="41" priority="68">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL64">
-    <cfRule type="expression" dxfId="40" priority="7">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C61">
-    <cfRule type="expression" dxfId="39" priority="64">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="expression" dxfId="38" priority="62">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH42:AM42">
-    <cfRule type="expression" dxfId="37" priority="60">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AI22:AM22">
-    <cfRule type="expression" dxfId="36" priority="58">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL51:AM51">
-    <cfRule type="expression" dxfId="35" priority="47">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM43:AO43">
-    <cfRule type="expression" dxfId="34" priority="10">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK43">
-    <cfRule type="expression" dxfId="33" priority="9">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL40:AM40 AL44:AM50 AL43">
-    <cfRule type="expression" dxfId="32" priority="52">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL5:AM9 AL35:AM39 AM61 AM64">
-    <cfRule type="expression" dxfId="31" priority="53">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL57:AM57 AL45:AM47 AL50:AM50">
-    <cfRule type="expression" dxfId="30" priority="51">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL52:AM56">
-    <cfRule type="expression" dxfId="29" priority="49">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL49:AM49">
-    <cfRule type="expression" dxfId="28" priority="48">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL61">
-    <cfRule type="expression" dxfId="27" priority="8">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AN30:AO30 AN10:AO13 AN15:AO19">
-    <cfRule type="expression" dxfId="26" priority="42">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AN23:AO28">
-    <cfRule type="expression" dxfId="25" priority="41">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AN20:AO21">
-    <cfRule type="expression" dxfId="24" priority="40">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AN32:AO32">
-    <cfRule type="expression" dxfId="23" priority="37">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AN33:AO34">
-    <cfRule type="expression" dxfId="22" priority="36">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AN31:AO31">
-    <cfRule type="expression" dxfId="21" priority="39">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AN41:AO41">
-    <cfRule type="expression" dxfId="20" priority="38">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AN42:AO42">
-    <cfRule type="expression" dxfId="19" priority="35">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AN22:AO22">
-    <cfRule type="expression" dxfId="18" priority="34">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AN51">
-    <cfRule type="expression" dxfId="17" priority="27">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AN44:AN50 AN40:AO40">
-    <cfRule type="expression" dxfId="16" priority="32">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AN5:AN9 AO8:AO9 AN35:AO39">
-    <cfRule type="expression" dxfId="15" priority="33">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AN57 AN45:AN47 AN50">
-    <cfRule type="expression" dxfId="14" priority="31">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AN52:AN56">
-    <cfRule type="expression" dxfId="13" priority="29">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AN49">
-    <cfRule type="expression" dxfId="12" priority="28">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AO5:AO7">
-    <cfRule type="expression" dxfId="11" priority="17">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AO44:AO50">
-    <cfRule type="expression" dxfId="10" priority="16">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AO57 AO45:AO47 AO50">
-    <cfRule type="expression" dxfId="9" priority="15">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AO51">
-    <cfRule type="expression" dxfId="8" priority="11">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AO52:AO56">
-    <cfRule type="expression" dxfId="7" priority="13">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AO49">
-    <cfRule type="expression" dxfId="6" priority="12">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D61">
-    <cfRule type="expression" dxfId="5" priority="6">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D64">
-    <cfRule type="expression" dxfId="4" priority="5">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH61">
-    <cfRule type="expression" dxfId="3" priority="4">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH64:AJ64">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AI61">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ61">
+  <conditionalFormatting sqref="D59">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>

</xml_diff>

<commit_message>
Updated lighting test JSON again to include test for 6-11
</commit_message>
<xml_diff>
--- a/rct229/ruletest_engine/ruletest_jsons/ruletest_spreadsheets/lighting_test_draft.xlsx
+++ b/rct229/ruletest_engine/ruletest_jsons/ruletest_spreadsheets/lighting_test_draft.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ruleset-checking-tool\rct229\ruletest_engine\ruletest_jsons\ruletest_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B3A744-4FB7-4072-AB49-C37CC84D0246}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{008F42FB-AC1B-46BA-83D6-ECE3EAC6A672}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{6D4BDC1E-634D-4FA4-9728-A76C548BE460}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6D4BDC1E-634D-4FA4-9728-A76C548BE460}"/>
   </bookViews>
   <sheets>
     <sheet name="TCDs" sheetId="4" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="164">
   <si>
     <t>appendix_g_section_id</t>
   </si>
@@ -457,12 +457,6 @@
     <t>e</t>
   </si>
   <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
     <t>JSON_PATH: surfaces[0]</t>
   </si>
   <si>
@@ -557,18 +551,6 @@
   </si>
   <si>
     <t>Lighting power for all spaces in the P-RMR exceeds the lighting power allowance for the building</t>
-  </si>
-  <si>
-    <t>b-21</t>
-  </si>
-  <si>
-    <t>c-22</t>
-  </si>
-  <si>
-    <t>b-24</t>
-  </si>
-  <si>
-    <t>c-25</t>
   </si>
 </sst>
 </file>
@@ -970,7 +952,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="188">
+  <dxfs count="183">
     <dxf>
       <fill>
         <patternFill>
@@ -1429,6 +1411,41 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
@@ -1436,41 +1453,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
@@ -1499,6 +1481,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
@@ -1506,13 +1495,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
@@ -1541,6 +1523,62 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
@@ -1548,62 +1586,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
@@ -1611,6 +1593,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
@@ -1618,13 +1607,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
@@ -1653,6 +1635,118 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
@@ -1660,118 +1754,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
@@ -1779,63 +1761,28 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2615,7 +2562,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="5" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G21" sqref="G21"/>
+      <selection pane="topRight" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2721,47 +2668,47 @@
       </c>
       <c r="W1" s="5" t="str">
         <f>"rule-"&amp;W2&amp;"-"&amp;W3&amp;"-"&amp;W4</f>
-        <v>rule-6-8-b-21</v>
+        <v>rule-6-8-b</v>
       </c>
       <c r="X1" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>rule-6-8-b-24</v>
+        <f>"rule-"&amp;X2&amp;"-"&amp;X3&amp;"-"&amp;X4</f>
+        <v>rule-6-8-c</v>
       </c>
       <c r="Y1" s="5" t="str">
         <f>"rule-"&amp;Y2&amp;"-"&amp;Y3&amp;"-"&amp;Y4</f>
-        <v>rule-6-8-c-22</v>
+        <v>rule-6-8-d</v>
       </c>
       <c r="Z1" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>rule-6-8-c-25</v>
+        <f>"rule-"&amp;Z2&amp;"-"&amp;Z3&amp;"-"&amp;Z4</f>
+        <v>rule-6-8-e</v>
       </c>
       <c r="AA1" s="5" t="str">
+        <f>"rule-"&amp;AA2&amp;"-"&amp;AA3&amp;"-"&amp;AA4</f>
+        <v>rule-6-11-a</v>
+      </c>
+      <c r="AB1" s="5" t="str">
+        <f>"rule-"&amp;AB2&amp;"-"&amp;AB3&amp;"-"&amp;AB4</f>
+        <v>rule-6-11-b</v>
+      </c>
+      <c r="AC1" s="5" t="str">
         <f t="shared" si="0"/>
         <v>rule-6-12-a</v>
       </c>
-      <c r="AB1" s="5" t="str">
+      <c r="AD1" s="5" t="str">
         <f t="shared" si="0"/>
         <v>rule-6-12-b</v>
       </c>
-      <c r="AC1" s="5" t="str">
+      <c r="AE1" s="5" t="str">
         <f t="shared" si="0"/>
         <v>rule-6-12-c</v>
       </c>
-      <c r="AD1" s="5" t="str">
+      <c r="AF1" s="5" t="str">
         <f t="shared" si="0"/>
         <v>rule-6-12-d</v>
       </c>
-      <c r="AE1" s="5" t="str">
+      <c r="AG1" s="5" t="str">
         <f t="shared" si="0"/>
         <v>rule-6-12-e</v>
-      </c>
-      <c r="AF1" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>rule-6-12-f</v>
-      </c>
-      <c r="AG1" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>rule-6-12-g</v>
       </c>
       <c r="AH1" s="5" t="str">
         <f t="shared" si="0"/>
@@ -2985,10 +2932,10 @@
         <v>8</v>
       </c>
       <c r="AA3" s="3">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AB3" s="3">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AC3" s="3">
         <v>12</v>
@@ -3090,16 +3037,16 @@
         <v>8</v>
       </c>
       <c r="W4" s="3" t="s">
-        <v>166</v>
+        <v>19</v>
       </c>
       <c r="X4" s="3" t="s">
-        <v>168</v>
+        <v>77</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>167</v>
+        <v>78</v>
       </c>
       <c r="Z4" s="3" t="s">
-        <v>169</v>
+        <v>131</v>
       </c>
       <c r="AA4" s="3" t="s">
         <v>8</v>
@@ -3108,19 +3055,19 @@
         <v>19</v>
       </c>
       <c r="AC4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE4" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="AD4" s="3" t="s">
+      <c r="AF4" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="AE4" s="3" t="s">
+      <c r="AG4" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="AF4" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="AG4" s="3" t="s">
-        <v>133</v>
       </c>
       <c r="AH4" s="3" t="s">
         <v>8</v>
@@ -3156,16 +3103,16 @@
       <c r="D5" s="12"/>
       <c r="E5" s="29"/>
       <c r="F5" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H5" s="4" t="s">
         <v>92</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J5" s="4" t="s">
         <v>93</v>
@@ -3207,61 +3154,61 @@
         <v>116</v>
       </c>
       <c r="W5" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="X5" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y5" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="X5" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="Y5" s="4" t="s">
+      <c r="Z5" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="Z5" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="AA5" s="46" t="s">
-        <v>125</v>
+      <c r="AA5" s="4" t="s">
+        <v>129</v>
       </c>
       <c r="AB5" s="4" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="AC5" s="46" t="s">
         <v>125</v>
       </c>
       <c r="AD5" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="AE5" s="46" t="s">
+        <v>125</v>
+      </c>
+      <c r="AF5" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="AE5" s="4" t="s">
+      <c r="AG5" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="AF5" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="AG5" s="4" t="s">
-        <v>130</v>
-      </c>
       <c r="AH5" s="46" t="s">
+        <v>145</v>
+      </c>
+      <c r="AI5" s="46" t="s">
+        <v>145</v>
+      </c>
+      <c r="AJ5" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="AK5" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="AI5" s="46" t="s">
-        <v>147</v>
-      </c>
-      <c r="AJ5" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="AK5" s="4" t="s">
-        <v>149</v>
-      </c>
       <c r="AL5" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="AM5" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="AN5" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="AM5" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="AN5" s="4" t="s">
-        <v>156</v>
-      </c>
       <c r="AO5" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:41" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3327,10 +3274,10 @@
         <v>5</v>
       </c>
       <c r="X6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y6" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="Y6" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="Z6" s="3" t="s">
         <v>20</v>
@@ -3339,22 +3286,22 @@
         <v>5</v>
       </c>
       <c r="AB6" s="3" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="AC6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="AD6" s="3" t="s">
-        <v>99</v>
+        <v>5</v>
       </c>
       <c r="AE6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="AF6" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="AG6" s="3" t="s">
         <v>5</v>
-      </c>
-      <c r="AG6" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="AH6" s="3" t="s">
         <v>99</v>
@@ -3503,28 +3450,28 @@
       <c r="X8" s="6"/>
       <c r="Y8" s="6"/>
       <c r="Z8" s="6"/>
-      <c r="AA8" s="6" t="str">
+      <c r="AA8" s="6"/>
+      <c r="AB8" s="6"/>
+      <c r="AC8" s="6" t="str">
         <f>"true"</f>
         <v>true</v>
       </c>
-      <c r="AB8" s="6" t="str">
+      <c r="AD8" s="6" t="str">
         <f>"true"</f>
         <v>true</v>
       </c>
-      <c r="AC8" s="6" t="str">
-        <f t="shared" ref="AC8:AE8" si="3">"true"</f>
+      <c r="AE8" s="6" t="str">
+        <f t="shared" ref="AE8:AG8" si="3">"true"</f>
         <v>true</v>
       </c>
-      <c r="AD8" s="6" t="str">
+      <c r="AF8" s="6" t="str">
         <f t="shared" si="3"/>
         <v>true</v>
       </c>
-      <c r="AE8" s="6" t="str">
+      <c r="AG8" s="6" t="str">
         <f t="shared" si="3"/>
         <v>true</v>
       </c>
-      <c r="AF8" s="6"/>
-      <c r="AG8" s="6"/>
       <c r="AH8" s="6" t="str">
         <f>"true"</f>
         <v>true</v>
@@ -3622,17 +3569,17 @@
         <f t="shared" si="5"/>
         <v>true</v>
       </c>
-      <c r="AA9" s="22"/>
-      <c r="AB9" s="22"/>
+      <c r="AA9" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB9" s="22" t="s">
+        <v>68</v>
+      </c>
       <c r="AC9" s="22"/>
       <c r="AD9" s="22"/>
       <c r="AE9" s="22"/>
-      <c r="AF9" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="AG9" s="22" t="s">
-        <v>68</v>
-      </c>
+      <c r="AF9" s="22"/>
+      <c r="AG9" s="22"/>
       <c r="AH9" s="22" t="s">
         <v>68</v>
       </c>
@@ -3919,11 +3866,11 @@
         <f>"true"</f>
         <v>true</v>
       </c>
-      <c r="X12" s="3" t="str">
+      <c r="W12" s="3" t="str">
         <f>"false"</f>
         <v>false</v>
       </c>
-      <c r="Z12" s="3" t="str">
+      <c r="X12" s="3" t="str">
         <f>"true"</f>
         <v>true</v>
       </c>
@@ -4066,112 +4013,112 @@
       </c>
       <c r="E14" s="29"/>
       <c r="F14" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="P14" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="R14" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="S14" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="T14" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="U14" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="V14" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="W14" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="X14" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="Y14" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="Z14" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="AA14" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="AB14" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="AC14" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="AD14" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="AE14" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="AF14" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="AG14" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="AH14" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="AI14" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="AJ14" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="AK14" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="AL14" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="AM14" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="AN14" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="AO14" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.25">
@@ -4969,28 +4916,28 @@
       </c>
       <c r="E22" s="29"/>
       <c r="F22" s="35" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G22" s="35" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H22" s="35" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I22" s="35" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J22" s="35" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="K22" s="35" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="L22" s="35" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="M22" s="35" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="N22" s="27" t="s">
         <v>79</v>
@@ -5012,16 +4959,16 @@
         <v>111</v>
       </c>
       <c r="W22" s="27" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="X22" s="27" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="Y22" s="27" t="s">
         <v>105</v>
       </c>
       <c r="Z22" s="27" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="AA22" s="27"/>
       <c r="AB22" s="27"/>
@@ -5037,10 +4984,10 @@
         <v>111</v>
       </c>
       <c r="AJ22" s="27" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="AK22" s="27" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="AL22" s="27" t="s">
         <v>111</v>
@@ -5052,7 +4999,7 @@
         <v>111</v>
       </c>
       <c r="AO22" s="27" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="23" spans="1:41" x14ac:dyDescent="0.25">
@@ -5196,10 +5143,10 @@
       <c r="V24" s="3" t="s">
         <v>115</v>
       </c>
+      <c r="W24" s="3" t="s">
+        <v>120</v>
+      </c>
       <c r="X24" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="Z24" s="3" t="s">
         <v>115</v>
       </c>
     </row>
@@ -5561,61 +5508,61 @@
         <v>113</v>
       </c>
       <c r="W30" s="3" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="X30" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="Y30" s="3" t="s">
         <v>103</v>
       </c>
       <c r="Z30" s="3" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="AA30" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="AB30" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="AC30" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="AD30" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="AE30" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="AF30" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="AG30" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="AH30" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="AI30" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="AJ30" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="AK30" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="AL30" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="AM30" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="AN30" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="AO30" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:41" x14ac:dyDescent="0.25">
@@ -5680,16 +5627,16 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="W31" s="3">
+        <v>1.2</v>
+      </c>
+      <c r="X31" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="Y31" s="3">
         <v>2.1</v>
       </c>
-      <c r="X31" s="3">
-        <v>1.2</v>
-      </c>
-      <c r="Y31" s="3">
+      <c r="Z31" s="3">
         <v>2.4</v>
-      </c>
-      <c r="Z31" s="3" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="32" spans="1:41" x14ac:dyDescent="0.25">
@@ -5706,7 +5653,7 @@
         <v>84</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K32" s="33"/>
       <c r="U32" s="32"/>
@@ -5723,12 +5670,12 @@
         <v>false</v>
       </c>
       <c r="AD32" s="3" t="str">
+        <f>"true"</f>
+        <v>true</v>
+      </c>
+      <c r="AE32" s="3" t="str">
         <f>"false"</f>
         <v>false</v>
-      </c>
-      <c r="AE32" s="3" t="str">
-        <f>"true"</f>
-        <v>true</v>
       </c>
       <c r="AF32" s="3" t="str">
         <f>"false"</f>
@@ -5753,7 +5700,7 @@
         <v>84</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="K33" s="33"/>
       <c r="U33" s="32"/>
@@ -5788,33 +5735,33 @@
         <v>84</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="K34" s="33"/>
       <c r="U34" s="32"/>
       <c r="AH34" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="AI34" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="AJ34" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="AK34" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="AL34" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="AM34" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="AN34" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="AO34" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="35" spans="1:41" x14ac:dyDescent="0.25">
@@ -5851,10 +5798,10 @@
       <c r="Q35" s="3">
         <v>2</v>
       </c>
-      <c r="W35" s="3">
+      <c r="Y35" s="3">
         <v>2</v>
       </c>
-      <c r="Y35" s="3">
+      <c r="Z35" s="3">
         <v>2</v>
       </c>
     </row>
@@ -5892,10 +5839,10 @@
       <c r="Q36" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="W36" s="3" t="s">
+      <c r="Y36" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="Y36" s="3" t="s">
+      <c r="Z36" s="3" t="s">
         <v>104</v>
       </c>
     </row>
@@ -5933,10 +5880,10 @@
       <c r="Q37" s="3">
         <v>0.32</v>
       </c>
-      <c r="W37" s="3">
+      <c r="Y37" s="3">
         <v>2.1</v>
       </c>
-      <c r="Y37" s="3">
+      <c r="Z37" s="3">
         <v>2.1</v>
       </c>
     </row>
@@ -6083,7 +6030,7 @@
         <v>61</v>
       </c>
       <c r="C41" s="38" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D41" s="38" t="s">
         <v>63</v>
@@ -6150,7 +6097,7 @@
         <v>61</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D42" s="12" t="s">
         <v>65</v>
@@ -6185,28 +6132,28 @@
       <c r="AF42" s="25"/>
       <c r="AG42" s="25"/>
       <c r="AH42" s="25" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="AI42" s="25" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="AJ42" s="25" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="AK42" s="25" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="AL42" s="25" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="AM42" s="25" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="AN42" s="25" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="AO42" s="25" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="43" spans="1:41" s="26" customFormat="1" x14ac:dyDescent="0.25">
@@ -6217,10 +6164,10 @@
         <v>61</v>
       </c>
       <c r="C43" s="42" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D43" s="42" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E43" s="43"/>
       <c r="F43" s="44"/>
@@ -6280,7 +6227,7 @@
         <v>61</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D44" s="12" t="s">
         <v>63</v>
@@ -6345,7 +6292,7 @@
         <v>61</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D45" s="12" t="s">
         <v>65</v>
@@ -6373,25 +6320,25 @@
       <c r="Y45" s="25"/>
       <c r="Z45" s="25"/>
       <c r="AA45" s="25" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="AB45" s="25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AC45" s="25" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AD45" s="25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AE45" s="25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AF45" s="25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AG45" s="25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AH45" s="25"/>
       <c r="AI45" s="25"/>
@@ -6410,10 +6357,10 @@
         <v>61</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E46" s="12"/>
       <c r="F46" s="25"/>
@@ -6438,25 +6385,25 @@
       <c r="Y46" s="25"/>
       <c r="Z46" s="25"/>
       <c r="AA46" s="25" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AB46" s="25" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AC46" s="25" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AD46" s="25" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AE46" s="25" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AF46" s="25" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AG46" s="25" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AH46" s="25"/>
       <c r="AI46" s="25"/>
@@ -6475,10 +6422,10 @@
         <v>61</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D47" s="36" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E47" s="12"/>
       <c r="F47" s="25"/>
@@ -6540,10 +6487,10 @@
         <v>61</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E48" s="12"/>
       <c r="F48" s="25"/>
@@ -6568,25 +6515,25 @@
       <c r="Y48" s="25"/>
       <c r="Z48" s="25"/>
       <c r="AA48" s="25">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="AB48" s="25" t="s">
         <v>122</v>
       </c>
       <c r="AC48" s="25">
+        <v>0</v>
+      </c>
+      <c r="AD48" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="AE48" s="25">
         <v>180</v>
       </c>
-      <c r="AD48" s="25">
+      <c r="AF48" s="25">
         <v>1</v>
       </c>
-      <c r="AE48" s="25">
-        <v>0</v>
-      </c>
-      <c r="AF48" s="25">
-        <v>180</v>
-      </c>
-      <c r="AG48" s="25" t="s">
-        <v>122</v>
+      <c r="AG48" s="25">
+        <v>0</v>
       </c>
       <c r="AH48" s="25"/>
       <c r="AI48" s="25"/>
@@ -6605,10 +6552,10 @@
         <v>61</v>
       </c>
       <c r="C49" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D49" s="36" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E49" s="12" t="s">
         <v>63</v>
@@ -6635,16 +6582,16 @@
       <c r="Y49" s="25"/>
       <c r="Z49" s="25"/>
       <c r="AA49" s="25"/>
-      <c r="AB49" s="25" t="s">
-        <v>122</v>
-      </c>
+      <c r="AB49" s="25"/>
       <c r="AC49" s="25"/>
-      <c r="AD49" s="25"/>
-      <c r="AE49" s="25" t="s">
-        <v>122</v>
-      </c>
+      <c r="AD49" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="AE49" s="25"/>
       <c r="AF49" s="25"/>
-      <c r="AG49" s="25"/>
+      <c r="AG49" s="25" t="s">
+        <v>122</v>
+      </c>
       <c r="AH49" s="25"/>
       <c r="AI49" s="25"/>
       <c r="AJ49" s="25"/>
@@ -6662,10 +6609,10 @@
         <v>61</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D50" s="36" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E50" s="12" t="s">
         <v>65</v>
@@ -6692,16 +6639,16 @@
       <c r="Y50" s="25"/>
       <c r="Z50" s="25"/>
       <c r="AA50" s="25"/>
-      <c r="AB50" s="25" t="s">
-        <v>146</v>
-      </c>
+      <c r="AB50" s="25"/>
       <c r="AC50" s="25"/>
-      <c r="AD50" s="25"/>
-      <c r="AE50" s="25" t="s">
-        <v>146</v>
-      </c>
+      <c r="AD50" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="AE50" s="25"/>
       <c r="AF50" s="25"/>
-      <c r="AG50" s="25"/>
+      <c r="AG50" s="25" t="s">
+        <v>144</v>
+      </c>
       <c r="AH50" s="25"/>
       <c r="AI50" s="25"/>
       <c r="AJ50" s="25"/>
@@ -6719,25 +6666,25 @@
         <v>61</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D51" s="36" t="s">
         <v>63</v>
       </c>
       <c r="E51" s="12"/>
+      <c r="AA51" s="3">
+        <v>2</v>
+      </c>
       <c r="AB51" s="3">
         <v>2</v>
       </c>
-      <c r="AC51" s="3">
-        <v>2</v>
-      </c>
       <c r="AD51" s="3">
         <v>2</v>
       </c>
+      <c r="AE51" s="3">
+        <v>2</v>
+      </c>
       <c r="AF51" s="3">
-        <v>2</v>
-      </c>
-      <c r="AG51" s="3">
         <v>2</v>
       </c>
     </row>
@@ -6749,26 +6696,26 @@
         <v>61</v>
       </c>
       <c r="C52" s="12" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D52" s="12" t="s">
         <v>65</v>
       </c>
       <c r="E52" s="12"/>
+      <c r="AA52" s="3" t="s">
+        <v>142</v>
+      </c>
       <c r="AB52" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="AC52" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="AD52" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
+      </c>
+      <c r="AE52" s="3" t="s">
+        <v>142</v>
       </c>
       <c r="AF52" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="AG52" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="53" spans="1:41" x14ac:dyDescent="0.25">
@@ -6779,26 +6726,26 @@
         <v>61</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E53" s="12"/>
+      <c r="AA53" s="3" t="s">
+        <v>158</v>
+      </c>
       <c r="AB53" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="AC53" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="AD53" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
+      </c>
+      <c r="AE53" s="3" t="s">
+        <v>158</v>
       </c>
       <c r="AF53" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="AG53" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="54" spans="1:41" x14ac:dyDescent="0.25">
@@ -6809,25 +6756,25 @@
         <v>61</v>
       </c>
       <c r="C54" s="12" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D54" s="36" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E54" s="12"/>
+      <c r="AA54" s="3">
+        <v>90</v>
+      </c>
       <c r="AB54" s="3">
         <v>90</v>
       </c>
-      <c r="AC54" s="3">
-        <v>90</v>
-      </c>
       <c r="AD54" s="3">
         <v>90</v>
       </c>
+      <c r="AE54" s="3">
+        <v>90</v>
+      </c>
       <c r="AF54" s="3">
-        <v>90</v>
-      </c>
-      <c r="AG54" s="3">
         <v>90</v>
       </c>
     </row>
@@ -6839,25 +6786,25 @@
         <v>61</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E55" s="12"/>
+      <c r="AA55" s="3">
+        <v>270</v>
+      </c>
       <c r="AB55" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="AC55" s="3">
+      <c r="AD55" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="AE55" s="3">
         <v>180</v>
       </c>
-      <c r="AD55" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="AF55" s="3">
-        <v>270</v>
-      </c>
-      <c r="AG55" s="3" t="s">
+      <c r="AF55" s="3" t="s">
         <v>122</v>
       </c>
     </row>
@@ -6869,15 +6816,15 @@
         <v>61</v>
       </c>
       <c r="C56" s="12" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D56" s="36" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E56" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="AB56" s="3">
+      <c r="AD56" s="3">
         <v>2</v>
       </c>
     </row>
@@ -6889,10 +6836,10 @@
         <v>61</v>
       </c>
       <c r="C57" s="21" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D57" s="45" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E57" s="21" t="s">
         <v>65</v>
@@ -6919,11 +6866,11 @@
       <c r="Y57" s="22"/>
       <c r="Z57" s="22"/>
       <c r="AA57" s="22"/>
-      <c r="AB57" s="22" t="s">
-        <v>145</v>
-      </c>
+      <c r="AB57" s="22"/>
       <c r="AC57" s="22"/>
-      <c r="AD57" s="22"/>
+      <c r="AD57" s="22" t="s">
+        <v>143</v>
+      </c>
       <c r="AE57" s="22"/>
       <c r="AF57" s="22"/>
       <c r="AG57" s="22"/>
@@ -6969,10 +6916,10 @@
         <v>13</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D59" s="42" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E59" s="29"/>
       <c r="F59" s="6"/>
@@ -7064,10 +7011,10 @@
         <v>12</v>
       </c>
       <c r="C62" s="12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D62" s="42" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E62" s="29"/>
       <c r="F62" s="6"/>
@@ -7173,10 +7120,10 @@
         <v>11</v>
       </c>
       <c r="C65" s="12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D65" s="42" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E65" s="29"/>
       <c r="F65" s="6"/>
@@ -7335,617 +7282,602 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A67:E78 A5:E5 A10:E19">
-    <cfRule type="expression" dxfId="187" priority="285">
+    <cfRule type="expression" dxfId="182" priority="285">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="expression" dxfId="186" priority="260">
+    <cfRule type="expression" dxfId="181" priority="260">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:E6">
-    <cfRule type="expression" dxfId="185" priority="259">
+    <cfRule type="expression" dxfId="180" priority="259">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="expression" dxfId="184" priority="257">
+    <cfRule type="expression" dxfId="179" priority="257">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:E9">
-    <cfRule type="expression" dxfId="183" priority="256">
+    <cfRule type="expression" dxfId="178" priority="256">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="expression" dxfId="180" priority="258">
+    <cfRule type="expression" dxfId="177" priority="258">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="expression" dxfId="179" priority="214">
+    <cfRule type="expression" dxfId="176" priority="214">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:B9">
-    <cfRule type="expression" dxfId="178" priority="243">
+    <cfRule type="expression" dxfId="175" priority="243">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:E24">
-    <cfRule type="expression" dxfId="177" priority="254">
+    <cfRule type="expression" dxfId="174" priority="254">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22:E22">
-    <cfRule type="expression" dxfId="176" priority="245">
+    <cfRule type="expression" dxfId="173" priority="245">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D63:E63">
-    <cfRule type="expression" dxfId="175" priority="206">
+    <cfRule type="expression" dxfId="172" priority="206">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29:B30 A23:B24">
-    <cfRule type="expression" dxfId="174" priority="244">
+    <cfRule type="expression" dxfId="171" priority="244">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22:B22">
-    <cfRule type="expression" dxfId="173" priority="240">
+    <cfRule type="expression" dxfId="170" priority="240">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31:B34">
-    <cfRule type="expression" dxfId="172" priority="241">
+    <cfRule type="expression" dxfId="169" priority="241">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C24 C29:C37">
-    <cfRule type="expression" dxfId="171" priority="238">
+    <cfRule type="expression" dxfId="168" priority="238">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58:B59">
-    <cfRule type="expression" dxfId="170" priority="239">
+    <cfRule type="expression" dxfId="167" priority="239">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25:E26">
-    <cfRule type="expression" dxfId="169" priority="235">
+    <cfRule type="expression" dxfId="166" priority="235">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D28:E28">
-    <cfRule type="expression" dxfId="168" priority="234">
+    <cfRule type="expression" dxfId="165" priority="234">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27:E27">
-    <cfRule type="expression" dxfId="167" priority="233">
+    <cfRule type="expression" dxfId="164" priority="233">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:B28 A25:B26">
-    <cfRule type="expression" dxfId="166" priority="232">
+    <cfRule type="expression" dxfId="163" priority="232">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A27:B27">
-    <cfRule type="expression" dxfId="165" priority="231">
+    <cfRule type="expression" dxfId="162" priority="231">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25:C28">
-    <cfRule type="expression" dxfId="164" priority="230">
+    <cfRule type="expression" dxfId="161" priority="230">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D38:D39">
-    <cfRule type="expression" dxfId="163" priority="229">
+    <cfRule type="expression" dxfId="160" priority="229">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D61">
-    <cfRule type="expression" dxfId="162" priority="193">
+    <cfRule type="expression" dxfId="159" priority="193">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D38:D39">
-    <cfRule type="expression" dxfId="161" priority="228">
+    <cfRule type="expression" dxfId="158" priority="228">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:B39">
-    <cfRule type="expression" dxfId="160" priority="226">
+    <cfRule type="expression" dxfId="157" priority="226">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38:C39">
-    <cfRule type="expression" dxfId="159" priority="224">
+    <cfRule type="expression" dxfId="156" priority="224">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E38:E39">
-    <cfRule type="expression" dxfId="158" priority="223">
+    <cfRule type="expression" dxfId="155" priority="223">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29">
-    <cfRule type="expression" dxfId="157" priority="217">
+    <cfRule type="expression" dxfId="154" priority="217">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E38">
-    <cfRule type="expression" dxfId="156" priority="222">
+    <cfRule type="expression" dxfId="153" priority="222">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29:D34">
-    <cfRule type="expression" dxfId="155" priority="220">
+    <cfRule type="expression" dxfId="152" priority="220">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D29:D34">
-    <cfRule type="expression" dxfId="154" priority="219">
+    <cfRule type="expression" dxfId="151" priority="219">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29:E30">
-    <cfRule type="expression" dxfId="153" priority="218">
+    <cfRule type="expression" dxfId="150" priority="218">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E31:E34">
-    <cfRule type="expression" dxfId="152" priority="216">
+    <cfRule type="expression" dxfId="149" priority="216">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E65">
-    <cfRule type="expression" dxfId="151" priority="204">
+    <cfRule type="expression" dxfId="148" priority="204">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D60:E60">
-    <cfRule type="expression" dxfId="150" priority="213">
+    <cfRule type="expression" dxfId="147" priority="213">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A60:B60">
-    <cfRule type="expression" dxfId="149" priority="212">
+    <cfRule type="expression" dxfId="146" priority="212">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E62">
-    <cfRule type="expression" dxfId="148" priority="211">
+    <cfRule type="expression" dxfId="145" priority="211">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A61:B62">
-    <cfRule type="expression" dxfId="147" priority="209">
+    <cfRule type="expression" dxfId="144" priority="209">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A62:B62">
-    <cfRule type="expression" dxfId="146" priority="208">
+    <cfRule type="expression" dxfId="143" priority="208">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63">
-    <cfRule type="expression" dxfId="145" priority="207">
+    <cfRule type="expression" dxfId="142" priority="207">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A63:B63">
-    <cfRule type="expression" dxfId="144" priority="205">
+    <cfRule type="expression" dxfId="141" priority="205">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A64:B65">
-    <cfRule type="expression" dxfId="143" priority="202">
+    <cfRule type="expression" dxfId="140" priority="202">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A65:B65">
-    <cfRule type="expression" dxfId="142" priority="201">
+    <cfRule type="expression" dxfId="139" priority="201">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C66">
-    <cfRule type="expression" dxfId="141" priority="200">
+    <cfRule type="expression" dxfId="138" priority="200">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D66:E66">
-    <cfRule type="expression" dxfId="140" priority="199">
+    <cfRule type="expression" dxfId="137" priority="199">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A66">
-    <cfRule type="expression" dxfId="139" priority="198">
+    <cfRule type="expression" dxfId="136" priority="198">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D64">
-    <cfRule type="expression" dxfId="138" priority="188">
+    <cfRule type="expression" dxfId="135" priority="188">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E64">
-    <cfRule type="expression" dxfId="137" priority="187">
+    <cfRule type="expression" dxfId="134" priority="187">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B66">
-    <cfRule type="expression" dxfId="136" priority="195">
+    <cfRule type="expression" dxfId="133" priority="195">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61">
-    <cfRule type="expression" dxfId="135" priority="194">
+    <cfRule type="expression" dxfId="132" priority="194">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37:B37">
-    <cfRule type="expression" dxfId="134" priority="183">
+    <cfRule type="expression" dxfId="131" priority="183">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D61">
-    <cfRule type="expression" dxfId="133" priority="192">
+    <cfRule type="expression" dxfId="130" priority="192">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E61">
-    <cfRule type="expression" dxfId="132" priority="191">
+    <cfRule type="expression" dxfId="129" priority="191">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C64">
-    <cfRule type="expression" dxfId="131" priority="190">
+    <cfRule type="expression" dxfId="128" priority="190">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D64">
-    <cfRule type="expression" dxfId="130" priority="189">
+    <cfRule type="expression" dxfId="127" priority="189">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A52:B53">
-    <cfRule type="expression" dxfId="129" priority="122">
+    <cfRule type="expression" dxfId="126" priority="122">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A54:B55">
-    <cfRule type="expression" dxfId="128" priority="121">
+    <cfRule type="expression" dxfId="125" priority="121">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35:D37">
-    <cfRule type="expression" dxfId="127" priority="186">
+    <cfRule type="expression" dxfId="124" priority="186">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D35:D37">
-    <cfRule type="expression" dxfId="126" priority="185">
+    <cfRule type="expression" dxfId="123" priority="185">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A35:B36">
-    <cfRule type="expression" dxfId="125" priority="184">
+    <cfRule type="expression" dxfId="122" priority="184">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="expression" dxfId="124" priority="180">
+    <cfRule type="expression" dxfId="121" priority="180">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35:E36">
-    <cfRule type="expression" dxfId="123" priority="181">
+    <cfRule type="expression" dxfId="120" priority="181">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37">
-    <cfRule type="expression" dxfId="122" priority="179">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F35:K38 AA22 AH30:AM30 AA10:AM13 AN58:AO65 AK62 AK65 V35:Z43 V58:AM61 V66:AO78 V63:AM64 V62:AG62 V65:AG65 V22:Z28 V5:Z13 V15:AM21 V14:AO14 V51:Z57 V42:AG42 V43:AJ43 V44:AK50 F39:U50 N35:U38 N51:U56 W35:W78 W5:W28 R35:U78 Y35:Y78 F30:AG34 Y5:Y28 F5:U28 F57:U78">
-    <cfRule type="expression" dxfId="121" priority="176">
+    <cfRule type="expression" dxfId="119" priority="179">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F35:K38 AH30:AM30 AN58:AO65 AK62 AK65 F39:U50 N35:U38 N51:U56 F57:U78 AH10:AM13 AH58:AM61 AH66:AO78 AH63:AM64 AH15:AM21 AH14:AO14 AH43:AJ43 AH44:AK50 F30:AB34 AC30:AG50 AC5:AG22 F5:AB28 AA23:AM28 AC56:AG78 AG52:AG55 R35:AB78 AA51:AG51">
+    <cfRule type="expression" dxfId="118" priority="176">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40:C43">
-    <cfRule type="expression" dxfId="120" priority="175">
+    <cfRule type="expression" dxfId="117" priority="175">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D40:E43">
-    <cfRule type="expression" dxfId="119" priority="174">
+    <cfRule type="expression" dxfId="116" priority="174">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40:B43">
-    <cfRule type="expression" dxfId="118" priority="173">
+    <cfRule type="expression" dxfId="115" priority="173">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L35:M36">
-    <cfRule type="expression" dxfId="117" priority="171">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA40:AG43">
-    <cfRule type="expression" dxfId="116" priority="167">
+    <cfRule type="expression" dxfId="114" priority="171">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L37:M38">
-    <cfRule type="expression" dxfId="115" priority="169">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA35:AG39 AA5:AG9 AB22:AG22 AA23:AM28">
-    <cfRule type="expression" dxfId="114" priority="168">
+    <cfRule type="expression" dxfId="113" priority="169">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A44:B44">
-    <cfRule type="expression" dxfId="113" priority="166">
+    <cfRule type="expression" dxfId="112" priority="166">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44:C48 C50">
-    <cfRule type="expression" dxfId="112" priority="165">
+    <cfRule type="expression" dxfId="111" priority="165">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20:E21">
-    <cfRule type="expression" dxfId="111" priority="137">
+    <cfRule type="expression" dxfId="110" priority="137">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50:B50">
-    <cfRule type="expression" dxfId="110" priority="162">
+    <cfRule type="expression" dxfId="109" priority="162">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52:C57">
-    <cfRule type="expression" dxfId="109" priority="133">
+    <cfRule type="expression" dxfId="108" priority="133">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56:B57">
-    <cfRule type="expression" dxfId="108" priority="130">
+    <cfRule type="expression" dxfId="107" priority="130">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D44">
-    <cfRule type="expression" dxfId="107" priority="158">
+    <cfRule type="expression" dxfId="106" priority="158">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D44">
-    <cfRule type="expression" dxfId="106" priority="157">
+    <cfRule type="expression" dxfId="105" priority="157">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44">
-    <cfRule type="expression" dxfId="105" priority="156">
+    <cfRule type="expression" dxfId="104" priority="156">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47:B48">
-    <cfRule type="expression" dxfId="104" priority="152">
+    <cfRule type="expression" dxfId="103" priority="152">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45:D46 D48">
-    <cfRule type="expression" dxfId="103" priority="155">
+    <cfRule type="expression" dxfId="102" priority="155">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45:D46 D48">
-    <cfRule type="expression" dxfId="102" priority="154">
+    <cfRule type="expression" dxfId="101" priority="154">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A45:B46">
-    <cfRule type="expression" dxfId="101" priority="153">
+    <cfRule type="expression" dxfId="100" priority="153">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E45">
-    <cfRule type="expression" dxfId="100" priority="150">
+    <cfRule type="expression" dxfId="99" priority="150">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E45:E46">
-    <cfRule type="expression" dxfId="99" priority="151">
+    <cfRule type="expression" dxfId="98" priority="151">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E47:E48">
-    <cfRule type="expression" dxfId="98" priority="149">
+    <cfRule type="expression" dxfId="97" priority="149">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F45:K48 F50:K50">
-    <cfRule type="expression" dxfId="97" priority="148">
+    <cfRule type="expression" dxfId="96" priority="148">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L45:M46">
-    <cfRule type="expression" dxfId="96" priority="143">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA45:AD47 AA48 AC48:AD48">
-    <cfRule type="expression" dxfId="95" priority="138">
+    <cfRule type="expression" dxfId="95" priority="143">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC45:AF47 AC48 AE48:AF48">
+    <cfRule type="expression" dxfId="94" priority="138">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L47:M48 L50:M50">
-    <cfRule type="expression" dxfId="94" priority="142">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA57:AG57 AA50:AD50 AF45:AG47 AF50:AG50 AF48">
-    <cfRule type="expression" dxfId="93" priority="141">
+    <cfRule type="expression" dxfId="93" priority="142">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA45:AB47 AA50:AF50 AA48">
+    <cfRule type="expression" dxfId="92" priority="141">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D47">
-    <cfRule type="expression" dxfId="92" priority="139">
+    <cfRule type="expression" dxfId="91" priority="139">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH22">
-    <cfRule type="expression" dxfId="91" priority="66">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB52:AD54 AC55">
-    <cfRule type="expression" dxfId="90" priority="110">
+    <cfRule type="expression" dxfId="90" priority="66">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD52:AF54 AE55">
+    <cfRule type="expression" dxfId="89" priority="110">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="expression" dxfId="89" priority="109">
+    <cfRule type="expression" dxfId="88" priority="109">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49:B49">
-    <cfRule type="expression" dxfId="88" priority="106">
+    <cfRule type="expression" dxfId="87" priority="106">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D49:D50">
-    <cfRule type="expression" dxfId="87" priority="100">
+    <cfRule type="expression" dxfId="86" priority="100">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D52:D53 D55">
-    <cfRule type="expression" dxfId="86" priority="124">
+    <cfRule type="expression" dxfId="85" priority="124">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D52:D53 D55">
-    <cfRule type="expression" dxfId="85" priority="123">
+    <cfRule type="expression" dxfId="84" priority="123">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52">
-    <cfRule type="expression" dxfId="84" priority="119">
+    <cfRule type="expression" dxfId="83" priority="119">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52:E53">
-    <cfRule type="expression" dxfId="83" priority="120">
+    <cfRule type="expression" dxfId="82" priority="120">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E54:E55">
-    <cfRule type="expression" dxfId="82" priority="118">
+    <cfRule type="expression" dxfId="81" priority="118">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F52:K56">
-    <cfRule type="expression" dxfId="81" priority="117">
+    <cfRule type="expression" dxfId="80" priority="117">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L52:M53">
-    <cfRule type="expression" dxfId="80" priority="116">
+    <cfRule type="expression" dxfId="79" priority="116">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH51:AK51">
-    <cfRule type="expression" dxfId="79" priority="74">
+    <cfRule type="expression" dxfId="78" priority="74">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L54:M56">
-    <cfRule type="expression" dxfId="78" priority="115">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA56:AF56 AE52:AF55 AG52:AG56">
-    <cfRule type="expression" dxfId="77" priority="114">
+    <cfRule type="expression" dxfId="77" priority="115">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB52:AB56">
+    <cfRule type="expression" dxfId="76" priority="114">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D54">
-    <cfRule type="expression" dxfId="76" priority="113">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA52:AA55">
-    <cfRule type="expression" dxfId="75" priority="111">
+    <cfRule type="expression" dxfId="75" priority="113">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC52:AC55">
+    <cfRule type="expression" dxfId="74" priority="111">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH32:AM32">
-    <cfRule type="expression" dxfId="74" priority="73">
+    <cfRule type="expression" dxfId="73" priority="73">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F49:K49">
-    <cfRule type="expression" dxfId="73" priority="103">
+    <cfRule type="expression" dxfId="72" priority="103">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L49:M49">
-    <cfRule type="expression" dxfId="72" priority="102">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA49 AC49:AD49 AF49:AG49">
-    <cfRule type="expression" dxfId="71" priority="101">
+    <cfRule type="expression" dxfId="71" priority="102">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE49:AF49 AA49:AC49">
+    <cfRule type="expression" dxfId="70" priority="101">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49:E50">
-    <cfRule type="expression" dxfId="70" priority="99">
+    <cfRule type="expression" dxfId="69" priority="99">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D56:D57">
-    <cfRule type="expression" dxfId="69" priority="98">
+    <cfRule type="expression" dxfId="68" priority="98">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E56:E57">
-    <cfRule type="expression" dxfId="68" priority="97">
+    <cfRule type="expression" dxfId="67" priority="97">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C51">
-    <cfRule type="expression" dxfId="67" priority="96">
+    <cfRule type="expression" dxfId="66" priority="96">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A51:B51">
-    <cfRule type="expression" dxfId="66" priority="95">
+    <cfRule type="expression" dxfId="65" priority="95">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F51:K51">
-    <cfRule type="expression" dxfId="65" priority="94">
+    <cfRule type="expression" dxfId="64" priority="94">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L51:M51">
-    <cfRule type="expression" dxfId="64" priority="93">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AA51:AG51">
-    <cfRule type="expression" dxfId="63" priority="92">
+    <cfRule type="expression" dxfId="63" priority="93">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7959,12 +7891,12 @@
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE45:AE48">
+  <conditionalFormatting sqref="AG45:AG48">
     <cfRule type="expression" dxfId="60" priority="89">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE50">
+  <conditionalFormatting sqref="AG50">
     <cfRule type="expression" dxfId="59" priority="88">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
@@ -7974,22 +7906,22 @@
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB49">
+  <conditionalFormatting sqref="AD49">
     <cfRule type="expression" dxfId="57" priority="86">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB55">
+  <conditionalFormatting sqref="AD55">
     <cfRule type="expression" dxfId="56" priority="85">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD55">
+  <conditionalFormatting sqref="AF55">
     <cfRule type="expression" dxfId="55" priority="84">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE49">
+  <conditionalFormatting sqref="AG49">
     <cfRule type="expression" dxfId="54" priority="83">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>

</xml_diff>

<commit_message>
Added schedule capabilities and made minor adjustments to lighting test json. Test JSON not yet finished.
</commit_message>
<xml_diff>
--- a/rct229/ruletest_engine/ruletest_jsons/ruletest_spreadsheets/lighting_test_draft.xlsx
+++ b/rct229/ruletest_engine/ruletest_jsons/ruletest_spreadsheets/lighting_test_draft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ruleset-checking-tool\rct229\ruletest_engine\ruletest_jsons\ruletest_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDAA0DF0-436F-4953-B441-F63D7832876A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BAC0B0C-A34E-4464-8622-FB86E9A23008}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{6D4BDC1E-634D-4FA4-9728-A76C548BE460}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="166">
   <si>
     <t>appendix_g_section_id</t>
   </si>
@@ -550,7 +550,13 @@
     <t>NA</t>
   </si>
   <si>
-    <t>OpenSchedule1</t>
+    <t>SCHEDULE:LIBRARY-Office_Occupancy</t>
+  </si>
+  <si>
+    <t>Always On Schedule</t>
+  </si>
+  <si>
+    <t>Office Schedule</t>
   </si>
 </sst>
 </file>
@@ -610,7 +616,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -644,6 +650,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -832,7 +844,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -942,11 +954,42 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="185">
+  <dxfs count="189">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2569,10 +2612,10 @@
   <dimension ref="A1:AM78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="V22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="V2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V42" sqref="V42"/>
+      <selection pane="bottomRight" activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2802,13 +2845,13 @@
       <c r="U2" s="3">
         <v>6</v>
       </c>
-      <c r="V2" s="3">
+      <c r="V2" s="45">
         <v>6</v>
       </c>
-      <c r="W2" s="3">
+      <c r="W2" s="45">
         <v>6</v>
       </c>
-      <c r="X2" s="3">
+      <c r="X2" s="45">
         <v>6</v>
       </c>
       <c r="Y2" s="3">
@@ -2913,13 +2956,13 @@
       <c r="U3" s="3">
         <v>8</v>
       </c>
-      <c r="V3" s="3">
+      <c r="V3" s="45">
         <v>9</v>
       </c>
-      <c r="W3" s="3">
+      <c r="W3" s="45">
         <v>9</v>
       </c>
-      <c r="X3" s="3">
+      <c r="X3" s="45">
         <v>9</v>
       </c>
       <c r="Y3" s="3">
@@ -3024,13 +3067,13 @@
       <c r="U4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="V4" s="3" t="s">
+      <c r="V4" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="W4" s="3" t="s">
+      <c r="W4" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="X4" s="3" t="s">
+      <c r="X4" s="45" t="s">
         <v>77</v>
       </c>
       <c r="Y4" s="3" t="s">
@@ -5904,13 +5947,13 @@
       <c r="T42" s="24"/>
       <c r="U42" s="24"/>
       <c r="V42" s="24" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="W42" s="24" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="X42" s="24" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="Y42" s="24"/>
       <c r="Z42" s="24"/>
@@ -5974,9 +6017,17 @@
       <c r="S43" s="42"/>
       <c r="T43" s="42"/>
       <c r="U43" s="42"/>
-      <c r="V43" s="42"/>
-      <c r="W43" s="42"/>
-      <c r="X43" s="42"/>
+      <c r="V43" s="42" t="s">
+        <v>163</v>
+      </c>
+      <c r="W43" s="42" t="str">
+        <f>"SCHEDULE:CONSTANT-1"</f>
+        <v>SCHEDULE:CONSTANT-1</v>
+      </c>
+      <c r="X43" s="42" t="str">
+        <f>"SCHEDULE:CONSTANT-1"</f>
+        <v>SCHEDULE:CONSTANT-1</v>
+      </c>
       <c r="Y43" s="42"/>
       <c r="Z43" s="42"/>
       <c r="AA43" s="42"/>
@@ -7034,926 +7085,946 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A67:E78 A5:E5 A10:E19">
-    <cfRule type="expression" dxfId="184" priority="287">
+    <cfRule type="expression" dxfId="188" priority="291">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="expression" dxfId="183" priority="262">
+    <cfRule type="expression" dxfId="187" priority="266">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6:E6">
-    <cfRule type="expression" dxfId="182" priority="261">
+    <cfRule type="expression" dxfId="186" priority="265">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="expression" dxfId="181" priority="259">
+    <cfRule type="expression" dxfId="185" priority="263">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:E9">
-    <cfRule type="expression" dxfId="180" priority="258">
+    <cfRule type="expression" dxfId="184" priority="262">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="expression" dxfId="179" priority="260">
+    <cfRule type="expression" dxfId="183" priority="264">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C60">
-    <cfRule type="expression" dxfId="178" priority="216">
+    <cfRule type="expression" dxfId="182" priority="220">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:B9">
-    <cfRule type="expression" dxfId="177" priority="245">
+    <cfRule type="expression" dxfId="181" priority="249">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D23:E24">
-    <cfRule type="expression" dxfId="176" priority="256">
+    <cfRule type="expression" dxfId="180" priority="260">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D22:E22">
+    <cfRule type="expression" dxfId="179" priority="251">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D63:E63">
+    <cfRule type="expression" dxfId="178" priority="212">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A29:B30 A23:B24">
+    <cfRule type="expression" dxfId="177" priority="250">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A22:B22">
+    <cfRule type="expression" dxfId="176" priority="246">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A31:B34">
     <cfRule type="expression" dxfId="175" priority="247">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D63:E63">
-    <cfRule type="expression" dxfId="174" priority="208">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A29:B30 A23:B24">
-    <cfRule type="expression" dxfId="173" priority="246">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A22:B22">
-    <cfRule type="expression" dxfId="172" priority="242">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A31:B34">
-    <cfRule type="expression" dxfId="171" priority="243">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C22:C24 C29:C37">
-    <cfRule type="expression" dxfId="170" priority="240">
+    <cfRule type="expression" dxfId="174" priority="244">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A58:B59">
-    <cfRule type="expression" dxfId="169" priority="241">
+    <cfRule type="expression" dxfId="173" priority="245">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D25:E26">
+    <cfRule type="expression" dxfId="172" priority="241">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D28:E28">
+    <cfRule type="expression" dxfId="171" priority="240">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D27:E27">
+    <cfRule type="expression" dxfId="170" priority="239">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A28:B28 A25:B26">
+    <cfRule type="expression" dxfId="169" priority="238">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A27:B27">
     <cfRule type="expression" dxfId="168" priority="237">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D28:E28">
+  <conditionalFormatting sqref="C25:C28">
     <cfRule type="expression" dxfId="167" priority="236">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D27:E27">
+  <conditionalFormatting sqref="D38:D39">
     <cfRule type="expression" dxfId="166" priority="235">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A28:B28 A25:B26">
-    <cfRule type="expression" dxfId="165" priority="234">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A27:B27">
-    <cfRule type="expression" dxfId="164" priority="233">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C25:C28">
+  <conditionalFormatting sqref="D61">
+    <cfRule type="expression" dxfId="165" priority="199">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38:D39">
+    <cfRule type="expression" dxfId="164" priority="234">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A38:B39">
     <cfRule type="expression" dxfId="163" priority="232">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D38:D39">
-    <cfRule type="expression" dxfId="162" priority="231">
+  <conditionalFormatting sqref="C38:C39">
+    <cfRule type="expression" dxfId="162" priority="230">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E38:E39">
+    <cfRule type="expression" dxfId="161" priority="229">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E29">
+    <cfRule type="expression" dxfId="160" priority="223">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E38">
+    <cfRule type="expression" dxfId="159" priority="228">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D29:D34">
+    <cfRule type="expression" dxfId="158" priority="226">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D29:D34">
+    <cfRule type="expression" dxfId="157" priority="225">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E29:E30">
+    <cfRule type="expression" dxfId="156" priority="224">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31:E34">
+    <cfRule type="expression" dxfId="155" priority="222">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E65">
+    <cfRule type="expression" dxfId="154" priority="210">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D60:E60">
+    <cfRule type="expression" dxfId="153" priority="219">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A60:B60">
+    <cfRule type="expression" dxfId="152" priority="218">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E62">
+    <cfRule type="expression" dxfId="151" priority="217">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A61:B62">
+    <cfRule type="expression" dxfId="150" priority="215">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A62:B62">
+    <cfRule type="expression" dxfId="149" priority="214">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C63">
+    <cfRule type="expression" dxfId="148" priority="213">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A63:B63">
+    <cfRule type="expression" dxfId="147" priority="211">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A64:B65">
+    <cfRule type="expression" dxfId="146" priority="208">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A65:B65">
+    <cfRule type="expression" dxfId="145" priority="207">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C66">
+    <cfRule type="expression" dxfId="144" priority="206">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D66:E66">
+    <cfRule type="expression" dxfId="143" priority="205">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A66">
+    <cfRule type="expression" dxfId="142" priority="204">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D64">
+    <cfRule type="expression" dxfId="141" priority="194">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E64">
+    <cfRule type="expression" dxfId="140" priority="193">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B66">
+    <cfRule type="expression" dxfId="139" priority="201">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C61">
+    <cfRule type="expression" dxfId="138" priority="200">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A37:B37">
+    <cfRule type="expression" dxfId="137" priority="189">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D61">
-    <cfRule type="expression" dxfId="161" priority="195">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D38:D39">
-    <cfRule type="expression" dxfId="160" priority="230">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A38:B39">
-    <cfRule type="expression" dxfId="159" priority="228">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C39">
-    <cfRule type="expression" dxfId="158" priority="226">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E38:E39">
-    <cfRule type="expression" dxfId="157" priority="225">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E29">
-    <cfRule type="expression" dxfId="156" priority="219">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E38">
-    <cfRule type="expression" dxfId="155" priority="224">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D29:D34">
-    <cfRule type="expression" dxfId="154" priority="222">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D29:D34">
-    <cfRule type="expression" dxfId="153" priority="221">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E29:E30">
-    <cfRule type="expression" dxfId="152" priority="220">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E31:E34">
-    <cfRule type="expression" dxfId="151" priority="218">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E65">
-    <cfRule type="expression" dxfId="150" priority="206">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D60:E60">
-    <cfRule type="expression" dxfId="149" priority="215">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A60:B60">
-    <cfRule type="expression" dxfId="148" priority="214">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E62">
-    <cfRule type="expression" dxfId="147" priority="213">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A61:B62">
-    <cfRule type="expression" dxfId="146" priority="211">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A62:B62">
-    <cfRule type="expression" dxfId="145" priority="210">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
-    <cfRule type="expression" dxfId="144" priority="209">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A63:B63">
-    <cfRule type="expression" dxfId="143" priority="207">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A64:B65">
-    <cfRule type="expression" dxfId="142" priority="204">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A65:B65">
-    <cfRule type="expression" dxfId="141" priority="203">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C66">
-    <cfRule type="expression" dxfId="140" priority="202">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D66:E66">
-    <cfRule type="expression" dxfId="139" priority="201">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A66">
-    <cfRule type="expression" dxfId="138" priority="200">
+    <cfRule type="expression" dxfId="136" priority="198">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E61">
+    <cfRule type="expression" dxfId="135" priority="197">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C64">
+    <cfRule type="expression" dxfId="134" priority="196">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D64">
-    <cfRule type="expression" dxfId="137" priority="190">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E64">
-    <cfRule type="expression" dxfId="136" priority="189">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B66">
-    <cfRule type="expression" dxfId="135" priority="197">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C61">
-    <cfRule type="expression" dxfId="134" priority="196">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A37:B37">
-    <cfRule type="expression" dxfId="133" priority="185">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D61">
-    <cfRule type="expression" dxfId="132" priority="194">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E61">
-    <cfRule type="expression" dxfId="131" priority="193">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
+    <cfRule type="expression" dxfId="133" priority="195">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A52:B53">
+    <cfRule type="expression" dxfId="132" priority="128">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A54:B55">
+    <cfRule type="expression" dxfId="131" priority="127">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D35:D37">
     <cfRule type="expression" dxfId="130" priority="192">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D64">
+  <conditionalFormatting sqref="D35:D37">
     <cfRule type="expression" dxfId="129" priority="191">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A52:B53">
-    <cfRule type="expression" dxfId="128" priority="124">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A54:B55">
-    <cfRule type="expression" dxfId="127" priority="123">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D35:D37">
-    <cfRule type="expression" dxfId="126" priority="188">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D35:D37">
-    <cfRule type="expression" dxfId="125" priority="187">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A35:B36">
-    <cfRule type="expression" dxfId="124" priority="186">
+    <cfRule type="expression" dxfId="128" priority="190">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="expression" dxfId="123" priority="182">
+    <cfRule type="expression" dxfId="127" priority="186">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35:E36">
-    <cfRule type="expression" dxfId="122" priority="183">
+    <cfRule type="expression" dxfId="126" priority="187">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37">
-    <cfRule type="expression" dxfId="121" priority="181">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F35:I38 AF30:AK30 AL58:AM65 AI62 AI65 L35:S38 L51:S56 AF10:AK13 AF58:AK61 AF66:AM78 AF63:AK64 AF15:AK21 AF14:AM14 AF43:AH43 AF44:AI50 AA30:AE50 AA5:AE22 Y23:AK28 AA56:AE78 AE52:AE55 Y51:AE51 F39:S50 F57:S78 P35:Z40 F30:Z34 F5:Z28 P43:Z78 P41:U42 Y41:Z42">
-    <cfRule type="expression" dxfId="120" priority="178">
+    <cfRule type="expression" dxfId="125" priority="185">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F35:I38 AF30:AK30 AL58:AM65 AI62 AI65 L35:S38 L51:S56 AF10:AK13 AF58:AK61 AF66:AM78 AF63:AK64 AF15:AK21 AF14:AM14 AF43:AH43 AF44:AI50 AA30:AE50 AA5:AE22 Y23:AK28 AA56:AE78 AE52:AE55 Y51:AE51 F39:S50 F57:S78 P35:Z40 F30:Z34 F5:Z28 P44:Z78 P41:U43 Y41:Z43">
+    <cfRule type="expression" dxfId="124" priority="182">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40:C43">
-    <cfRule type="expression" dxfId="119" priority="177">
+    <cfRule type="expression" dxfId="123" priority="181">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D40:E43">
-    <cfRule type="expression" dxfId="118" priority="176">
+    <cfRule type="expression" dxfId="122" priority="180">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40:B43">
-    <cfRule type="expression" dxfId="117" priority="175">
+    <cfRule type="expression" dxfId="121" priority="179">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J35:K36">
-    <cfRule type="expression" dxfId="116" priority="173">
+    <cfRule type="expression" dxfId="120" priority="177">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J37:K38">
-    <cfRule type="expression" dxfId="115" priority="171">
+    <cfRule type="expression" dxfId="119" priority="175">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A44:B44">
-    <cfRule type="expression" dxfId="114" priority="168">
+    <cfRule type="expression" dxfId="118" priority="172">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C44:C48 C50">
-    <cfRule type="expression" dxfId="113" priority="167">
+    <cfRule type="expression" dxfId="117" priority="171">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20:E21">
-    <cfRule type="expression" dxfId="112" priority="139">
+    <cfRule type="expression" dxfId="116" priority="143">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A50:B50">
-    <cfRule type="expression" dxfId="111" priority="164">
+    <cfRule type="expression" dxfId="115" priority="168">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52:C57">
-    <cfRule type="expression" dxfId="110" priority="135">
+    <cfRule type="expression" dxfId="114" priority="139">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56:B57">
-    <cfRule type="expression" dxfId="109" priority="132">
+    <cfRule type="expression" dxfId="113" priority="136">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D44">
-    <cfRule type="expression" dxfId="108" priority="160">
+    <cfRule type="expression" dxfId="112" priority="164">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D44">
-    <cfRule type="expression" dxfId="107" priority="159">
+    <cfRule type="expression" dxfId="111" priority="163">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E44">
-    <cfRule type="expression" dxfId="106" priority="158">
+    <cfRule type="expression" dxfId="110" priority="162">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A47:B48">
-    <cfRule type="expression" dxfId="105" priority="154">
+    <cfRule type="expression" dxfId="109" priority="158">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45:D46 D48">
+    <cfRule type="expression" dxfId="108" priority="161">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D45:D46 D48">
+    <cfRule type="expression" dxfId="107" priority="160">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A45:B46">
+    <cfRule type="expression" dxfId="106" priority="159">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E45">
+    <cfRule type="expression" dxfId="105" priority="156">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E45:E46">
     <cfRule type="expression" dxfId="104" priority="157">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D45:D46 D48">
-    <cfRule type="expression" dxfId="103" priority="156">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A45:B46">
-    <cfRule type="expression" dxfId="102" priority="155">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E45">
-    <cfRule type="expression" dxfId="101" priority="152">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E45:E46">
-    <cfRule type="expression" dxfId="100" priority="153">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="E47:E48">
-    <cfRule type="expression" dxfId="99" priority="151">
+    <cfRule type="expression" dxfId="103" priority="155">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F45:I48 F50:I50">
-    <cfRule type="expression" dxfId="98" priority="150">
+    <cfRule type="expression" dxfId="102" priority="154">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J45:K46">
+    <cfRule type="expression" dxfId="101" priority="149">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA45:AD47 AA48 AC48:AD48">
+    <cfRule type="expression" dxfId="100" priority="144">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J47:K48 J50:K50">
+    <cfRule type="expression" dxfId="99" priority="148">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y45:Z47 Y50:AD50 Y48">
+    <cfRule type="expression" dxfId="98" priority="147">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D47">
     <cfRule type="expression" dxfId="97" priority="145">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA45:AD47 AA48 AC48:AD48">
-    <cfRule type="expression" dxfId="96" priority="140">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J47:K48 J50:K50">
-    <cfRule type="expression" dxfId="95" priority="144">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y45:Z47 Y50:AD50 Y48">
-    <cfRule type="expression" dxfId="94" priority="143">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D47">
-    <cfRule type="expression" dxfId="93" priority="141">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="AF22">
-    <cfRule type="expression" dxfId="92" priority="68">
+    <cfRule type="expression" dxfId="96" priority="72">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB52:AD54 AC55">
-    <cfRule type="expression" dxfId="91" priority="112">
+    <cfRule type="expression" dxfId="95" priority="116">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="expression" dxfId="90" priority="111">
+    <cfRule type="expression" dxfId="94" priority="115">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A49:B49">
-    <cfRule type="expression" dxfId="89" priority="108">
+    <cfRule type="expression" dxfId="93" priority="112">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D49:D50">
-    <cfRule type="expression" dxfId="88" priority="102">
+    <cfRule type="expression" dxfId="92" priority="106">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D52:D53 D55">
-    <cfRule type="expression" dxfId="87" priority="126">
+    <cfRule type="expression" dxfId="91" priority="130">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D52:D53 D55">
-    <cfRule type="expression" dxfId="86" priority="125">
+    <cfRule type="expression" dxfId="90" priority="129">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52">
-    <cfRule type="expression" dxfId="85" priority="121">
+    <cfRule type="expression" dxfId="89" priority="125">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E52:E53">
-    <cfRule type="expression" dxfId="84" priority="122">
+    <cfRule type="expression" dxfId="88" priority="126">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E54:E55">
-    <cfRule type="expression" dxfId="83" priority="120">
+    <cfRule type="expression" dxfId="87" priority="124">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F52:I56">
-    <cfRule type="expression" dxfId="82" priority="119">
+    <cfRule type="expression" dxfId="86" priority="123">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J52:K53">
-    <cfRule type="expression" dxfId="81" priority="118">
+    <cfRule type="expression" dxfId="85" priority="122">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF51:AI51">
-    <cfRule type="expression" dxfId="80" priority="76">
+    <cfRule type="expression" dxfId="84" priority="80">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J54:K56">
-    <cfRule type="expression" dxfId="79" priority="117">
+    <cfRule type="expression" dxfId="83" priority="121">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z52:Z56">
-    <cfRule type="expression" dxfId="78" priority="116">
+    <cfRule type="expression" dxfId="82" priority="120">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D54">
-    <cfRule type="expression" dxfId="77" priority="115">
+    <cfRule type="expression" dxfId="81" priority="119">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA52:AA55">
-    <cfRule type="expression" dxfId="76" priority="113">
+    <cfRule type="expression" dxfId="80" priority="117">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF32:AK32">
-    <cfRule type="expression" dxfId="75" priority="75">
+    <cfRule type="expression" dxfId="79" priority="79">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F49:I49">
-    <cfRule type="expression" dxfId="74" priority="105">
+    <cfRule type="expression" dxfId="78" priority="109">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J49:K49">
-    <cfRule type="expression" dxfId="73" priority="104">
+    <cfRule type="expression" dxfId="77" priority="108">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC49:AD49 Y49:AA49">
-    <cfRule type="expression" dxfId="72" priority="103">
+    <cfRule type="expression" dxfId="76" priority="107">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49:E50">
+    <cfRule type="expression" dxfId="75" priority="105">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D56:D57">
+    <cfRule type="expression" dxfId="74" priority="104">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E56:E57">
+    <cfRule type="expression" dxfId="73" priority="103">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C51">
+    <cfRule type="expression" dxfId="72" priority="102">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A51:B51">
     <cfRule type="expression" dxfId="71" priority="101">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D56:D57">
+  <conditionalFormatting sqref="F51:I51">
     <cfRule type="expression" dxfId="70" priority="100">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E56:E57">
+  <conditionalFormatting sqref="J51:K51">
     <cfRule type="expression" dxfId="69" priority="99">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
-    <cfRule type="expression" dxfId="68" priority="98">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A51:B51">
-    <cfRule type="expression" dxfId="67" priority="97">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F51:I51">
-    <cfRule type="expression" dxfId="66" priority="96">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J51:K51">
-    <cfRule type="expression" dxfId="65" priority="95">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="D51">
-    <cfRule type="expression" dxfId="64" priority="93">
+    <cfRule type="expression" dxfId="68" priority="97">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
+    <cfRule type="expression" dxfId="67" priority="96">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE45:AE48">
+    <cfRule type="expression" dxfId="66" priority="95">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE50">
+    <cfRule type="expression" dxfId="65" priority="94">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF33:AK34">
+    <cfRule type="expression" dxfId="64" priority="78">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB49">
     <cfRule type="expression" dxfId="63" priority="92">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE45:AE48">
+  <conditionalFormatting sqref="AB55">
     <cfRule type="expression" dxfId="62" priority="91">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AE50">
+  <conditionalFormatting sqref="AD55">
     <cfRule type="expression" dxfId="61" priority="90">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF33:AK34">
-    <cfRule type="expression" dxfId="60" priority="74">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB49">
+  <conditionalFormatting sqref="AE49">
+    <cfRule type="expression" dxfId="60" priority="89">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF31:AK31">
     <cfRule type="expression" dxfId="59" priority="88">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB55">
-    <cfRule type="expression" dxfId="58" priority="87">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD55">
-    <cfRule type="expression" dxfId="57" priority="86">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE49">
+  <conditionalFormatting sqref="AF40:AI41 AJ41:AK41">
+    <cfRule type="expression" dxfId="58" priority="86">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF5:AI9 AF35:AI39">
+    <cfRule type="expression" dxfId="57" priority="87">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF57:AI57 AF45:AI47 AF50:AI50">
     <cfRule type="expression" dxfId="56" priority="85">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF31:AK31">
-    <cfRule type="expression" dxfId="55" priority="84">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF40:AI41 AJ41:AK41">
-    <cfRule type="expression" dxfId="54" priority="82">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF5:AI9 AF35:AI39">
-    <cfRule type="expression" dxfId="53" priority="83">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF57:AI57 AF45:AI47 AF50:AI50">
-    <cfRule type="expression" dxfId="52" priority="81">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="AF52:AI56">
-    <cfRule type="expression" dxfId="51" priority="78">
+    <cfRule type="expression" dxfId="55" priority="82">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF49:AI49">
-    <cfRule type="expression" dxfId="50" priority="77">
+    <cfRule type="expression" dxfId="54" priority="81">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ65">
-    <cfRule type="expression" dxfId="49" priority="16">
+    <cfRule type="expression" dxfId="53" priority="20">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="expression" dxfId="48" priority="73">
+    <cfRule type="expression" dxfId="52" priority="77">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C65">
-    <cfRule type="expression" dxfId="47" priority="71">
+    <cfRule type="expression" dxfId="51" priority="75">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF42:AK42">
-    <cfRule type="expression" dxfId="46" priority="69">
+    <cfRule type="expression" dxfId="50" priority="73">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG22:AK22">
-    <cfRule type="expression" dxfId="45" priority="67">
+    <cfRule type="expression" dxfId="49" priority="71">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ51:AK51">
-    <cfRule type="expression" dxfId="44" priority="56">
+    <cfRule type="expression" dxfId="48" priority="60">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK43:AM43">
-    <cfRule type="expression" dxfId="43" priority="19">
+    <cfRule type="expression" dxfId="47" priority="23">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI43">
-    <cfRule type="expression" dxfId="42" priority="18">
+    <cfRule type="expression" dxfId="46" priority="22">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ40:AK40 AJ44:AK50 AJ43">
+    <cfRule type="expression" dxfId="45" priority="65">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ5:AK9 AJ35:AK39 AK62 AK65">
+    <cfRule type="expression" dxfId="44" priority="66">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ57:AK57 AJ45:AK47 AJ50:AK50">
+    <cfRule type="expression" dxfId="43" priority="64">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ52:AK56">
+    <cfRule type="expression" dxfId="42" priority="62">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AJ49:AK49">
     <cfRule type="expression" dxfId="41" priority="61">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AJ5:AK9 AJ35:AK39 AK62 AK65">
-    <cfRule type="expression" dxfId="40" priority="62">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ57:AK57 AJ45:AK47 AJ50:AK50">
-    <cfRule type="expression" dxfId="39" priority="60">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ52:AK56">
-    <cfRule type="expression" dxfId="38" priority="58">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ49:AK49">
-    <cfRule type="expression" dxfId="37" priority="57">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="AJ62">
-    <cfRule type="expression" dxfId="36" priority="17">
+    <cfRule type="expression" dxfId="40" priority="21">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL30:AM30 AL10:AM13 AL15:AM19">
-    <cfRule type="expression" dxfId="35" priority="51">
+    <cfRule type="expression" dxfId="39" priority="55">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL23:AM28">
-    <cfRule type="expression" dxfId="34" priority="50">
+    <cfRule type="expression" dxfId="38" priority="54">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL20:AM21">
-    <cfRule type="expression" dxfId="33" priority="49">
+    <cfRule type="expression" dxfId="37" priority="53">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL32:AM32">
-    <cfRule type="expression" dxfId="32" priority="46">
+    <cfRule type="expression" dxfId="36" priority="50">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL33:AM34">
-    <cfRule type="expression" dxfId="31" priority="45">
+    <cfRule type="expression" dxfId="35" priority="49">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL31:AM31">
-    <cfRule type="expression" dxfId="30" priority="48">
+    <cfRule type="expression" dxfId="34" priority="52">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL41:AM41">
-    <cfRule type="expression" dxfId="29" priority="47">
+    <cfRule type="expression" dxfId="33" priority="51">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL42:AM42">
-    <cfRule type="expression" dxfId="28" priority="44">
+    <cfRule type="expression" dxfId="32" priority="48">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL22:AM22">
-    <cfRule type="expression" dxfId="27" priority="43">
+    <cfRule type="expression" dxfId="31" priority="47">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL51">
-    <cfRule type="expression" dxfId="26" priority="36">
+    <cfRule type="expression" dxfId="30" priority="40">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL44:AL50 AL40:AM40">
+    <cfRule type="expression" dxfId="29" priority="45">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL5:AL9 AM8:AM9 AL35:AM39">
+    <cfRule type="expression" dxfId="28" priority="46">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL57 AL45:AL47 AL50">
+    <cfRule type="expression" dxfId="27" priority="44">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL52:AL56">
+    <cfRule type="expression" dxfId="26" priority="42">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AL49">
     <cfRule type="expression" dxfId="25" priority="41">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AL5:AL9 AM8:AM9 AL35:AM39">
-    <cfRule type="expression" dxfId="24" priority="42">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL57 AL45:AL47 AL50">
-    <cfRule type="expression" dxfId="23" priority="40">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL52:AL56">
-    <cfRule type="expression" dxfId="22" priority="38">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AL49">
-    <cfRule type="expression" dxfId="21" priority="37">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="AM5:AM7">
+    <cfRule type="expression" dxfId="24" priority="30">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM44:AM50">
+    <cfRule type="expression" dxfId="23" priority="29">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM57 AM45:AM47 AM50">
+    <cfRule type="expression" dxfId="22" priority="28">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM51">
+    <cfRule type="expression" dxfId="21" priority="24">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AM52:AM56">
     <cfRule type="expression" dxfId="20" priority="26">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AM44:AM50">
+  <conditionalFormatting sqref="AM49">
     <cfRule type="expression" dxfId="19" priority="25">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AM57 AM45:AM47 AM50">
-    <cfRule type="expression" dxfId="18" priority="24">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM51">
-    <cfRule type="expression" dxfId="17" priority="20">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM52:AM56">
-    <cfRule type="expression" dxfId="16" priority="22">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AM49">
-    <cfRule type="expression" dxfId="15" priority="21">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="D62">
+    <cfRule type="expression" dxfId="18" priority="19">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D65">
+    <cfRule type="expression" dxfId="17" priority="18">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF62">
+    <cfRule type="expression" dxfId="16" priority="17">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF65:AH65">
+    <cfRule type="expression" dxfId="15" priority="16">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG62">
     <cfRule type="expression" dxfId="14" priority="15">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D65">
+  <conditionalFormatting sqref="AH62">
     <cfRule type="expression" dxfId="13" priority="14">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AF62">
-    <cfRule type="expression" dxfId="12" priority="13">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF65:AH65">
-    <cfRule type="expression" dxfId="11" priority="12">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG62">
-    <cfRule type="expression" dxfId="10" priority="11">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH62">
+  <conditionalFormatting sqref="D58">
+    <cfRule type="expression" dxfId="12" priority="11">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E59">
+    <cfRule type="expression" dxfId="11" priority="13">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C58">
+    <cfRule type="expression" dxfId="10" priority="12">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D58">
     <cfRule type="expression" dxfId="9" priority="10">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D58">
-    <cfRule type="expression" dxfId="8" priority="7">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E59">
-    <cfRule type="expression" dxfId="7" priority="9">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C58">
-    <cfRule type="expression" dxfId="6" priority="8">
-      <formula>MOD(ROW(),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D58">
+  <conditionalFormatting sqref="E58">
+    <cfRule type="expression" dxfId="8" priority="9">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D59">
+    <cfRule type="expression" dxfId="6" priority="7">
+      <formula>MOD(ROW(),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="V41:X41">
     <cfRule type="expression" dxfId="5" priority="6">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E58">
+  <conditionalFormatting sqref="V42:W42">
     <cfRule type="expression" dxfId="4" priority="5">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
+  <conditionalFormatting sqref="V43">
     <cfRule type="expression" dxfId="3" priority="4">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D59">
+  <conditionalFormatting sqref="W43">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V41:X41">
+  <conditionalFormatting sqref="X42">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="V42:X42">
+  <conditionalFormatting sqref="X43">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>

</xml_diff>

<commit_message>
Forgot a python script and some other files. Small correction for black formatting.
</commit_message>
<xml_diff>
--- a/rct229/ruletest_engine/ruletest_jsons/ruletest_spreadsheets/lighting_test_draft.xlsx
+++ b/rct229/ruletest_engine/ruletest_jsons/ruletest_spreadsheets/lighting_test_draft.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ruleset-checking-tool\rct229\ruletest_engine\ruletest_jsons\ruletest_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BAC0B0C-A34E-4464-8622-FB86E9A23008}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202CB4B0-5CB6-4E7E-BE60-971EE6A59131}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{6D4BDC1E-634D-4FA4-9728-A76C548BE460}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="166">
   <si>
     <t>appendix_g_section_id</t>
   </si>
@@ -2612,10 +2612,10 @@
   <dimension ref="A1:AM78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="V2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W6" sqref="W6"/>
+      <selection pane="bottomRight" activeCell="V26" sqref="V26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4438,6 +4438,15 @@
       <c r="U18" s="3">
         <v>0</v>
       </c>
+      <c r="V18" s="3">
+        <v>0</v>
+      </c>
+      <c r="W18" s="3">
+        <v>0</v>
+      </c>
+      <c r="X18" s="3">
+        <v>0</v>
+      </c>
       <c r="Y18" s="3">
         <v>0</v>
       </c>
@@ -4544,6 +4553,15 @@
         <v>73</v>
       </c>
       <c r="U19" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="V19" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="W19" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="X19" s="3" t="s">
         <v>73</v>
       </c>
       <c r="Y19" s="3" t="s">
@@ -7404,7 +7422,7 @@
       <formula>MOD(ROW(),2)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F35:I38 AF30:AK30 AL58:AM65 AI62 AI65 L35:S38 L51:S56 AF10:AK13 AF58:AK61 AF66:AM78 AF63:AK64 AF15:AK21 AF14:AM14 AF43:AH43 AF44:AI50 AA30:AE50 AA5:AE22 Y23:AK28 AA56:AE78 AE52:AE55 Y51:AE51 F39:S50 F57:S78 P35:Z40 F30:Z34 F5:Z28 P44:Z78 P41:U43 Y41:Z43">
+  <conditionalFormatting sqref="F35:I38 AF30:AK30 AL58:AM65 AI62 AI65 L35:S38 L51:S56 AF10:AK13 AF58:AK61 AF66:AM78 AF63:AK64 AF15:AK21 AF14:AM14 AF43:AH43 AF44:AI50 AA30:AE50 AA5:AE22 Y23:AK28 AA56:AE78 AE52:AE55 Y51:AE51 F39:S50 F57:S78 P35:Z40 F30:Z34 P44:Z78 P41:U43 Y41:Z43 F5:Z28">
     <cfRule type="expression" dxfId="124" priority="182">
       <formula>MOD(ROW(),2)</formula>
     </cfRule>

</xml_diff>